<commit_message>
refact: implement tree as a STP parsing result
</commit_message>
<xml_diff>
--- a/src/mapstp/data/default-material-index.xlsx
+++ b/src/mapstp/data/default-material-index.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$N$389</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$389</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="523">
   <si>
     <t xml:space="preserve">mnemonic</t>
   </si>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">ITER_D_HTN8X3 v2.1 (VV, 8.2)</t>
   </si>
   <si>
-    <t xml:space="preserve">SXM</t>
+    <t xml:space="preserve">XM-19</t>
   </si>
   <si>
     <t xml:space="preserve">XM-19 VV (IWS)</t>
@@ -1297,7 +1297,7 @@
     <t xml:space="preserve">8.2</t>
   </si>
   <si>
-    <t xml:space="preserve">HTN8X3 v2.1</t>
+    <t xml:space="preserve">ITER_D_HTN8X3 v2.1</t>
   </si>
   <si>
     <t xml:space="preserve">WATER</t>
@@ -1548,6 +1548,9 @@
   </si>
   <si>
     <t xml:space="preserve">PF1/6 joints, copy of m110805 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B4C-0.7</t>
   </si>
   <si>
     <t xml:space="preserve">Materials IVVS port and internals</t>
@@ -1744,17 +1747,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N389"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="E376" activeCellId="0" sqref="E376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1774,7 +1777,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1925,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>100</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
         <v>101</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
         <v>102</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>103</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>104</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>105</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
         <v>106</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
         <v>108</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
         <v>109</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
         <v>110</v>
       </c>
@@ -2243,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <v>112</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>113</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
         <v>120</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
         <v>121</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
         <v>122</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
         <v>123</v>
       </c>
@@ -2429,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
         <v>124</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
         <v>125</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
         <v>190</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
         <v>200</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
         <v>201</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
         <v>202</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
         <v>250</v>
       </c>
@@ -2678,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
         <v>251</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="n">
         <v>252</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="n">
         <v>253</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="n">
         <v>254</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="n">
         <v>301</v>
       </c>
@@ -2831,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="n">
         <v>302</v>
       </c>
@@ -2855,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
         <v>303</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="n">
         <v>306</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="n">
         <v>350</v>
       </c>
@@ -2991,6 +2994,9 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="B45" s="0" t="n">
         <v>400</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="n">
         <v>906</v>
       </c>
@@ -3038,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="n">
         <v>907</v>
       </c>
@@ -3059,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="n">
         <v>999</v>
       </c>
@@ -3080,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
         <v>9126</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="n">
         <v>97001</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="n">
         <v>107000</v>
       </c>
@@ -3158,7 +3164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="n">
         <v>150</v>
       </c>
@@ -3176,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="n">
         <v>151</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="n">
         <v>152</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="n">
         <v>153</v>
       </c>
@@ -3240,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="n">
         <v>351</v>
       </c>
@@ -3261,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
         <v>352</v>
       </c>
@@ -3279,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="n">
         <v>353</v>
       </c>
@@ -3297,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="n">
         <v>354</v>
       </c>
@@ -3315,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="n">
         <v>355</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="n">
         <v>356</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="n">
         <v>357</v>
       </c>
@@ -3375,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="n">
         <v>358</v>
       </c>
@@ -3399,7 +3405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="n">
         <v>359</v>
       </c>
@@ -3423,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="n">
         <v>360</v>
       </c>
@@ -3441,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="n">
         <v>361</v>
       </c>
@@ -3465,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="n">
         <v>362</v>
       </c>
@@ -3489,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="n">
         <v>363</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="n">
         <v>370</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="n">
         <v>371</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="n">
         <v>372</v>
       </c>
@@ -3576,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="n">
         <v>373</v>
       </c>
@@ -3597,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="n">
         <v>374</v>
       </c>
@@ -3618,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="n">
         <v>375</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="n">
         <v>376</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="n">
         <v>377</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="n">
         <v>378</v>
       </c>
@@ -3690,7 +3696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="n">
         <v>379</v>
       </c>
@@ -3711,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="n">
         <v>392</v>
       </c>
@@ -3732,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="n">
         <v>501</v>
       </c>
@@ -3756,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="n">
         <v>521</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="n">
         <v>541</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="n">
         <v>581</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="n">
         <v>2501</v>
       </c>
@@ -3852,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="n">
         <v>2521</v>
       </c>
@@ -3876,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="n">
         <v>2541</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="n">
         <v>2581</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="n">
         <v>4501</v>
       </c>
@@ -3948,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="n">
         <v>4521</v>
       </c>
@@ -3972,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="n">
         <v>4541</v>
       </c>
@@ -3996,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="n">
         <v>4581</v>
       </c>
@@ -4020,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="n">
         <v>502</v>
       </c>
@@ -4044,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="n">
         <v>522</v>
       </c>
@@ -4068,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="n">
         <v>542</v>
       </c>
@@ -4092,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="n">
         <v>582</v>
       </c>
@@ -4116,7 +4122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="n">
         <v>2502</v>
       </c>
@@ -4140,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="n">
         <v>2522</v>
       </c>
@@ -4164,7 +4170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="n">
         <v>2542</v>
       </c>
@@ -4188,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="n">
         <v>2582</v>
       </c>
@@ -4212,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="n">
         <v>4502</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="n">
         <v>4522</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="n">
         <v>4542</v>
       </c>
@@ -4284,7 +4290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="n">
         <v>4582</v>
       </c>
@@ -4308,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="n">
         <v>503</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="n">
         <v>523</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="n">
         <v>543</v>
       </c>
@@ -4380,7 +4386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="n">
         <v>583</v>
       </c>
@@ -4404,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="n">
         <v>2503</v>
       </c>
@@ -4428,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="n">
         <v>2523</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="n">
         <v>2543</v>
       </c>
@@ -4476,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="n">
         <v>2583</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="n">
         <v>4503</v>
       </c>
@@ -4524,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="n">
         <v>4523</v>
       </c>
@@ -4548,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="n">
         <v>4543</v>
       </c>
@@ -4572,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="n">
         <v>4583</v>
       </c>
@@ -4596,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="7" t="n">
         <v>504</v>
       </c>
@@ -4620,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="7" t="n">
         <v>524</v>
       </c>
@@ -4644,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="7" t="n">
         <v>544</v>
       </c>
@@ -4668,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="7" t="n">
         <v>584</v>
       </c>
@@ -4692,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="n">
         <v>2504</v>
       </c>
@@ -4716,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="n">
         <v>2524</v>
       </c>
@@ -4740,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="n">
         <v>2544</v>
       </c>
@@ -4764,7 +4770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="n">
         <v>2584</v>
       </c>
@@ -4788,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="n">
         <v>4504</v>
       </c>
@@ -4812,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="n">
         <v>4524</v>
       </c>
@@ -4836,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="n">
         <v>4544</v>
       </c>
@@ -4860,7 +4866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="n">
         <v>4584</v>
       </c>
@@ -4884,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="7" t="n">
         <v>505</v>
       </c>
@@ -4908,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="7" t="n">
         <v>525</v>
       </c>
@@ -4932,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="7" t="n">
         <v>545</v>
       </c>
@@ -4956,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="7" t="n">
         <v>585</v>
       </c>
@@ -4980,7 +4986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="n">
         <v>2505</v>
       </c>
@@ -5004,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="n">
         <v>2525</v>
       </c>
@@ -5028,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="n">
         <v>2545</v>
       </c>
@@ -5052,7 +5058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="n">
         <v>2585</v>
       </c>
@@ -5076,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="n">
         <v>4505</v>
       </c>
@@ -5100,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="n">
         <v>4525</v>
       </c>
@@ -5124,7 +5130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="n">
         <v>4545</v>
       </c>
@@ -5148,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="n">
         <v>4585</v>
       </c>
@@ -5172,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="7" t="n">
         <v>506</v>
       </c>
@@ -5196,7 +5202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="7" t="n">
         <v>526</v>
       </c>
@@ -5220,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="7" t="n">
         <v>546</v>
       </c>
@@ -5244,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="7" t="n">
         <v>586</v>
       </c>
@@ -5268,7 +5274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="n">
         <v>2506</v>
       </c>
@@ -5292,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="n">
         <v>2526</v>
       </c>
@@ -5316,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="n">
         <v>2546</v>
       </c>
@@ -5340,7 +5346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="0" t="n">
         <v>2586</v>
       </c>
@@ -5364,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="0" t="n">
         <v>4506</v>
       </c>
@@ -5388,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="0" t="n">
         <v>4526</v>
       </c>
@@ -5412,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="0" t="n">
         <v>4546</v>
       </c>
@@ -5436,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="0" t="n">
         <v>4586</v>
       </c>
@@ -5460,7 +5466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="0" t="n">
         <v>507</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="0" t="n">
         <v>527</v>
       </c>
@@ -5514,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="n">
         <v>547</v>
       </c>
@@ -5541,7 +5547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="0" t="n">
         <v>508</v>
       </c>
@@ -5568,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="0" t="n">
         <v>528</v>
       </c>
@@ -5595,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="0" t="n">
         <v>548</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="0" t="n">
         <v>509</v>
       </c>
@@ -5649,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="0" t="n">
         <v>529</v>
       </c>
@@ -5676,7 +5682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="0" t="n">
         <v>549</v>
       </c>
@@ -5703,7 +5709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="0" t="n">
         <v>567</v>
       </c>
@@ -5730,7 +5736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="0" t="n">
         <v>568</v>
       </c>
@@ -5757,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="0" t="n">
         <v>569</v>
       </c>
@@ -5784,7 +5790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="0" t="n">
         <v>587</v>
       </c>
@@ -5811,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="0" t="n">
         <v>588</v>
       </c>
@@ -5838,7 +5844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="0" t="n">
         <v>589</v>
       </c>
@@ -5865,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="0" t="n">
         <v>2507</v>
       </c>
@@ -5883,7 +5889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="0" t="n">
         <v>2527</v>
       </c>
@@ -5907,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="0" t="n">
         <v>2547</v>
       </c>
@@ -5931,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="0" t="n">
         <v>2508</v>
       </c>
@@ -5955,7 +5961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="0" t="n">
         <v>2528</v>
       </c>
@@ -5979,7 +5985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="0" t="n">
         <v>2548</v>
       </c>
@@ -6003,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="0" t="n">
         <v>2587</v>
       </c>
@@ -6027,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="0" t="n">
         <v>2588</v>
       </c>
@@ -6051,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="0" t="n">
         <v>2599</v>
       </c>
@@ -6075,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="n">
         <v>1510</v>
       </c>
@@ -6105,7 +6111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="0" t="n">
         <v>1530</v>
       </c>
@@ -6135,7 +6141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="0" t="n">
         <v>1550</v>
       </c>
@@ -6165,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="0" t="n">
         <v>1590</v>
       </c>
@@ -6195,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="0" t="n">
         <v>3511</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="0" t="n">
         <v>3531</v>
       </c>
@@ -6255,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="0" t="n">
         <v>3551</v>
       </c>
@@ -6285,7 +6291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="0" t="n">
         <v>3591</v>
       </c>
@@ -6315,7 +6321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="0" t="n">
         <v>2511</v>
       </c>
@@ -6345,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="0" t="n">
         <v>2531</v>
       </c>
@@ -6375,7 +6381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="n">
         <v>2551</v>
       </c>
@@ -6405,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="n">
         <v>2591</v>
       </c>
@@ -6435,7 +6441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="n">
         <v>1511</v>
       </c>
@@ -6459,7 +6465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="0" t="n">
         <v>1531</v>
       </c>
@@ -6483,7 +6489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="0" t="n">
         <v>1551</v>
       </c>
@@ -6507,7 +6513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="0" t="n">
         <v>1591</v>
       </c>
@@ -6531,7 +6537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="0" t="n">
         <v>511</v>
       </c>
@@ -6555,7 +6561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="0" t="n">
         <v>531</v>
       </c>
@@ -6579,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="0" t="n">
         <v>551</v>
       </c>
@@ -6603,7 +6609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="0" t="n">
         <v>591</v>
       </c>
@@ -6627,7 +6633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="0" t="n">
         <v>572</v>
       </c>
@@ -6651,7 +6657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="0" t="n">
         <v>592</v>
       </c>
@@ -6675,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="0" t="n">
         <v>512</v>
       </c>
@@ -6699,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="0" t="n">
         <v>532</v>
       </c>
@@ -6723,7 +6729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="0" t="n">
         <v>552</v>
       </c>
@@ -6747,7 +6753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="n">
         <v>3592</v>
       </c>
@@ -6771,7 +6777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="0" t="n">
         <v>2592</v>
       </c>
@@ -6795,7 +6801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="0" t="n">
         <v>1592</v>
       </c>
@@ -6819,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="0" t="n">
         <v>4513</v>
       </c>
@@ -6834,7 +6840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="0" t="n">
         <v>4533</v>
       </c>
@@ -6849,7 +6855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="0" t="n">
         <v>4553</v>
       </c>
@@ -6864,7 +6870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="n">
         <v>4593</v>
       </c>
@@ -6879,7 +6885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="0" t="n">
         <v>3513</v>
       </c>
@@ -6894,7 +6900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="n">
         <v>3533</v>
       </c>
@@ -6909,7 +6915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="0" t="n">
         <v>3553</v>
       </c>
@@ -6924,7 +6930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="0" t="n">
         <v>3593</v>
       </c>
@@ -6939,7 +6945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="n">
         <v>2513</v>
       </c>
@@ -6954,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="0" t="n">
         <v>2533</v>
       </c>
@@ -6969,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="0" t="n">
         <v>2553</v>
       </c>
@@ -6984,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="0" t="n">
         <v>2593</v>
       </c>
@@ -6999,7 +7005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="n">
         <v>1513</v>
       </c>
@@ -7014,7 +7020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="0" t="n">
         <v>1533</v>
       </c>
@@ -7029,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="0" t="n">
         <v>1553</v>
       </c>
@@ -7044,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="n">
         <v>1593</v>
       </c>
@@ -7059,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="n">
         <v>513</v>
       </c>
@@ -7074,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="0" t="n">
         <v>533</v>
       </c>
@@ -7089,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="n">
         <v>553</v>
       </c>
@@ -7104,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="n">
         <v>593</v>
       </c>
@@ -7119,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="n">
         <v>3514</v>
       </c>
@@ -7134,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="n">
         <v>3534</v>
       </c>
@@ -7149,7 +7155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="n">
         <v>3554</v>
       </c>
@@ -7164,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="n">
         <v>3594</v>
       </c>
@@ -7179,7 +7185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="n">
         <v>1514</v>
       </c>
@@ -7194,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="0" t="n">
         <v>1534</v>
       </c>
@@ -7209,7 +7215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="n">
         <v>1554</v>
       </c>
@@ -7224,7 +7230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="n">
         <v>1594</v>
       </c>
@@ -7239,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="n">
         <v>3515</v>
       </c>
@@ -7254,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="n">
         <v>3535</v>
       </c>
@@ -7269,7 +7275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="n">
         <v>3555</v>
       </c>
@@ -7284,7 +7290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="n">
         <v>3595</v>
       </c>
@@ -7299,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="n">
         <v>1515</v>
       </c>
@@ -7314,7 +7320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="n">
         <v>1535</v>
       </c>
@@ -7329,7 +7335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="n">
         <v>1555</v>
       </c>
@@ -7344,7 +7350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="n">
         <v>1595</v>
       </c>
@@ -7359,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="0" t="n">
         <v>4516</v>
       </c>
@@ -7374,7 +7380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="0" t="n">
         <v>4536</v>
       </c>
@@ -7389,7 +7395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="0" t="n">
         <v>4556</v>
       </c>
@@ -7404,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="0" t="n">
         <v>4596</v>
       </c>
@@ -7419,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="0" t="n">
         <v>3516</v>
       </c>
@@ -7434,7 +7440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="0" t="n">
         <v>3536</v>
       </c>
@@ -7449,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="0" t="n">
         <v>3556</v>
       </c>
@@ -7464,7 +7470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="0" t="n">
         <v>3596</v>
       </c>
@@ -7479,7 +7485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="0" t="n">
         <v>2516</v>
       </c>
@@ -7494,7 +7500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="0" t="n">
         <v>2536</v>
       </c>
@@ -7509,7 +7515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="0" t="n">
         <v>2556</v>
       </c>
@@ -7524,7 +7530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="0" t="n">
         <v>2596</v>
       </c>
@@ -7539,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="0" t="n">
         <v>1516</v>
       </c>
@@ -7554,7 +7560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="0" t="n">
         <v>1536</v>
       </c>
@@ -7569,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="0" t="n">
         <v>1556</v>
       </c>
@@ -7584,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="0" t="n">
         <v>1596</v>
       </c>
@@ -7599,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="n">
         <v>516</v>
       </c>
@@ -7614,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="0" t="n">
         <v>536</v>
       </c>
@@ -7629,7 +7635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="0" t="n">
         <v>556</v>
       </c>
@@ -7644,7 +7650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="0" t="n">
         <v>596</v>
       </c>
@@ -7659,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="0" t="n">
         <v>4517</v>
       </c>
@@ -7674,7 +7680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="0" t="n">
         <v>4537</v>
       </c>
@@ -7689,7 +7695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="0" t="n">
         <v>4557</v>
       </c>
@@ -7704,7 +7710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="0" t="n">
         <v>4597</v>
       </c>
@@ -7719,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="0" t="n">
         <v>3517</v>
       </c>
@@ -7734,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="0" t="n">
         <v>3537</v>
       </c>
@@ -7749,7 +7755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="0" t="n">
         <v>3557</v>
       </c>
@@ -7764,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="0" t="n">
         <v>3597</v>
       </c>
@@ -7779,7 +7785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="0" t="n">
         <v>2517</v>
       </c>
@@ -7794,7 +7800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="0" t="n">
         <v>2537</v>
       </c>
@@ -7809,7 +7815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="0" t="n">
         <v>2557</v>
       </c>
@@ -7824,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="0" t="n">
         <v>2597</v>
       </c>
@@ -7839,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="0" t="n">
         <v>1517</v>
       </c>
@@ -7854,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="0" t="n">
         <v>1537</v>
       </c>
@@ -7869,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="0" t="n">
         <v>1557</v>
       </c>
@@ -7884,7 +7890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="0" t="n">
         <v>1597</v>
       </c>
@@ -7899,7 +7905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="0" t="n">
         <v>517</v>
       </c>
@@ -7914,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="n">
         <v>537</v>
       </c>
@@ -7929,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="n">
         <v>557</v>
       </c>
@@ -7944,7 +7950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="n">
         <v>597</v>
       </c>
@@ -7959,7 +7965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="n">
         <v>4518</v>
       </c>
@@ -7974,7 +7980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="n">
         <v>4538</v>
       </c>
@@ -7989,7 +7995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="n">
         <v>4558</v>
       </c>
@@ -8004,7 +8010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="n">
         <v>4598</v>
       </c>
@@ -8019,7 +8025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="n">
         <v>3518</v>
       </c>
@@ -8034,7 +8040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="n">
         <v>3538</v>
       </c>
@@ -8049,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="n">
         <v>3558</v>
       </c>
@@ -8064,7 +8070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="n">
         <v>3598</v>
       </c>
@@ -8079,7 +8085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="n">
         <v>2518</v>
       </c>
@@ -8094,7 +8100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="n">
         <v>2538</v>
       </c>
@@ -8109,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="n">
         <v>2558</v>
       </c>
@@ -8124,7 +8130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="n">
         <v>2598</v>
       </c>
@@ -8139,7 +8145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="n">
         <v>1518</v>
       </c>
@@ -8154,7 +8160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="n">
         <v>1538</v>
       </c>
@@ -8169,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="n">
         <v>1558</v>
       </c>
@@ -8184,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="n">
         <v>1598</v>
       </c>
@@ -8199,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="n">
         <v>518</v>
       </c>
@@ -8214,7 +8220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="0" t="n">
         <v>538</v>
       </c>
@@ -8229,7 +8235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B298" s="0" t="n">
         <v>558</v>
       </c>
@@ -8244,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="0" t="n">
         <v>598</v>
       </c>
@@ -8259,7 +8265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="0" t="n">
         <v>6007</v>
       </c>
@@ -8271,7 +8277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="0" t="n">
         <v>6008</v>
       </c>
@@ -8283,7 +8289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="n">
         <v>6009</v>
       </c>
@@ -8295,7 +8301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="0" t="n">
         <v>6010</v>
       </c>
@@ -8307,7 +8313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B304" s="0" t="n">
         <v>7003</v>
       </c>
@@ -8319,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B305" s="0" t="n">
         <v>7004</v>
       </c>
@@ -8331,7 +8337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="0" t="n">
         <v>7005</v>
       </c>
@@ -8343,7 +8349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="0" t="n">
         <v>107001</v>
       </c>
@@ -8364,7 +8370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="0" t="n">
         <v>107002</v>
       </c>
@@ -8398,8 +8404,8 @@
       <c r="C309" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="E309" s="0" t="s">
-        <v>416</v>
+      <c r="E309" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="G309" s="0" t="s">
         <v>417</v>
@@ -8415,7 +8421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="0" t="n">
         <v>107004</v>
       </c>
@@ -8443,8 +8449,8 @@
       <c r="C311" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E311" s="0" t="s">
-        <v>412</v>
+      <c r="E311" s="0" t="n">
+        <v>7.93</v>
       </c>
       <c r="G311" s="0" t="s">
         <v>417</v>
@@ -8457,7 +8463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="0" t="n">
         <v>107006</v>
       </c>
@@ -8478,7 +8484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="0" t="n">
         <v>107007</v>
       </c>
@@ -8496,7 +8502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="n">
         <v>107009</v>
       </c>
@@ -8517,7 +8523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="0" t="n">
         <v>107301</v>
       </c>
@@ -8551,8 +8557,8 @@
       <c r="C316" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E316" s="0" t="s">
-        <v>412</v>
+      <c r="E316" s="0" t="n">
+        <v>7.93</v>
       </c>
       <c r="G316" s="0" t="s">
         <v>417</v>
@@ -8568,7 +8574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="0" t="n">
         <v>107303</v>
       </c>
@@ -8592,7 +8598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="0" t="n">
         <v>107304</v>
       </c>
@@ -8626,8 +8632,8 @@
       <c r="C319" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="E319" s="0" t="s">
-        <v>422</v>
+      <c r="E319" s="0" t="n">
+        <v>7.6</v>
       </c>
       <c r="G319" s="0" t="s">
         <v>417</v>
@@ -8640,7 +8646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="0" t="n">
         <v>107306</v>
       </c>
@@ -8661,7 +8667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="n">
         <v>107307</v>
       </c>
@@ -8679,7 +8685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="0" t="n">
         <v>107308</v>
       </c>
@@ -8697,7 +8703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="n">
         <v>107309</v>
       </c>
@@ -8718,7 +8724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="0" t="n">
         <v>107310</v>
       </c>
@@ -8739,7 +8745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="n">
         <v>107311</v>
       </c>
@@ -8754,7 +8760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="0" t="n">
         <v>107701</v>
       </c>
@@ -8778,7 +8784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="n">
         <v>107702</v>
       </c>
@@ -8802,7 +8808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="n">
         <v>107703</v>
       </c>
@@ -8823,7 +8829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="0" t="n">
         <v>108001</v>
       </c>
@@ -8847,7 +8853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="0" t="n">
         <v>108002</v>
       </c>
@@ -8871,7 +8877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="0" t="n">
         <v>108003</v>
       </c>
@@ -8892,7 +8898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B332" s="0" t="n">
         <v>108502</v>
       </c>
@@ -8910,7 +8916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B333" s="0" t="n">
         <v>108511</v>
       </c>
@@ -8931,7 +8937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="0" t="n">
         <v>108512</v>
       </c>
@@ -8952,7 +8958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="0" t="n">
         <v>108513</v>
       </c>
@@ -8973,7 +8979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="0" t="n">
         <v>108514</v>
       </c>
@@ -8994,7 +9000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B337" s="0" t="n">
         <v>108515</v>
       </c>
@@ -9015,7 +9021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B338" s="0" t="n">
         <v>108516</v>
       </c>
@@ -9036,7 +9042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B339" s="0" t="n">
         <v>108517</v>
       </c>
@@ -9057,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B340" s="0" t="n">
         <v>108518</v>
       </c>
@@ -9081,7 +9087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B341" s="0" t="n">
         <v>108519</v>
       </c>
@@ -9099,7 +9105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="0" t="n">
         <v>108520</v>
       </c>
@@ -9117,7 +9123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B343" s="0" t="n">
         <v>110501</v>
       </c>
@@ -9138,7 +9144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B344" s="0" t="n">
         <v>110502</v>
       </c>
@@ -9159,7 +9165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B345" s="0" t="n">
         <v>110503</v>
       </c>
@@ -9180,7 +9186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="0" t="n">
         <v>110504</v>
       </c>
@@ -9201,7 +9207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B347" s="0" t="n">
         <v>110505</v>
       </c>
@@ -9219,7 +9225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="0" t="n">
         <v>110506</v>
       </c>
@@ -9237,7 +9243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="56.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="56.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B349" s="0" t="n">
         <v>110507</v>
       </c>
@@ -9264,7 +9270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B350" s="0" t="n">
         <v>110801</v>
       </c>
@@ -9288,7 +9294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="34.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B351" s="0" t="n">
         <v>110802</v>
       </c>
@@ -9312,7 +9318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B352" s="0" t="n">
         <v>110803</v>
       </c>
@@ -9330,7 +9336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="67.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="67.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="0" t="n">
         <v>110804</v>
       </c>
@@ -9357,7 +9363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="89.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="89.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B354" s="0" t="n">
         <v>110805</v>
       </c>
@@ -9384,7 +9390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B355" s="0" t="n">
         <v>110901</v>
       </c>
@@ -9411,7 +9417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B356" s="0" t="n">
         <v>110902</v>
       </c>
@@ -9438,7 +9444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B357" s="0" t="n">
         <v>110903</v>
       </c>
@@ -9465,7 +9471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B358" s="0" t="n">
         <v>111101</v>
       </c>
@@ -9492,7 +9498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="0" t="n">
         <v>111102</v>
       </c>
@@ -9519,7 +9525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B360" s="0" t="n">
         <v>111103</v>
       </c>
@@ -9546,7 +9552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B361" s="0" t="n">
         <v>110851</v>
       </c>
@@ -9564,7 +9570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B362" s="0" t="n">
         <v>110852</v>
       </c>
@@ -9588,7 +9594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="89.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="89.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="0" t="n">
         <v>110853</v>
       </c>
@@ -9615,7 +9621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B364" s="0" t="n">
         <v>110951</v>
       </c>
@@ -9633,7 +9639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B365" s="0" t="n">
         <v>110952</v>
       </c>
@@ -9657,7 +9663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B366" s="0" t="n">
         <v>110953</v>
       </c>
@@ -9684,7 +9690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B367" s="0" t="n">
         <v>111151</v>
       </c>
@@ -9702,7 +9708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="0" t="n">
         <v>111152</v>
       </c>
@@ -9726,7 +9732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="0" t="n">
         <v>111153</v>
       </c>
@@ -9753,7 +9759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="0" t="n">
         <v>111251</v>
       </c>
@@ -9771,7 +9777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="0" t="n">
         <v>111252</v>
       </c>
@@ -9795,7 +9801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="0" t="n">
         <v>111253</v>
       </c>
@@ -9822,7 +9828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="0" t="n">
         <v>111351</v>
       </c>
@@ -9840,7 +9846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B374" s="0" t="n">
         <v>111352</v>
       </c>
@@ -9864,7 +9870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" customFormat="false" ht="89.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="89.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B375" s="0" t="n">
         <v>11353</v>
       </c>
@@ -9889,6 +9895,9 @@
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>502</v>
+      </c>
       <c r="B376" s="0" t="n">
         <v>114101</v>
       </c>
@@ -9905,7 +9914,7 @@
         <v>48</v>
       </c>
       <c r="L376" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="N376" s="5" t="n">
         <f aca="false">AND(E376 &gt; 0, K376 = "")</f>
@@ -9914,19 +9923,19 @@
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B377" s="0" t="n">
         <v>114102</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E377" s="0" t="n">
         <v>2.32</v>
       </c>
       <c r="L377" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="N377" s="5" t="n">
         <f aca="false">AND(E377 &gt; 0, K377 = "")</f>
@@ -9935,19 +9944,19 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B378" s="0" t="n">
         <v>114103</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E378" s="0" t="n">
         <v>7.7</v>
       </c>
       <c r="L378" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="N378" s="5" t="n">
         <f aca="false">AND(E378 &gt; 0, K378 = "")</f>
@@ -9956,31 +9965,31 @@
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B379" s="0" t="n">
         <v>114104</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E379" s="0" t="n">
         <v>3.97</v>
       </c>
       <c r="L379" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="N379" s="5" t="n">
         <f aca="false">AND(E379 &gt; 0, K379 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="0" t="n">
         <v>115100</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E380" s="0" t="n">
         <v>7.93</v>
@@ -9989,22 +9998,22 @@
         <v>0.086353</v>
       </c>
       <c r="G380" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L380" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="N380" s="5" t="n">
         <f aca="false">AND(E380 &gt; 0, K380 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="0" t="n">
         <v>115101</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E381" s="0" t="n">
         <v>2.7</v>
@@ -10013,22 +10022,22 @@
         <v>0.080544</v>
       </c>
       <c r="G381" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L381" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="N381" s="5" t="n">
         <f aca="false">AND(E381 &gt; 0, K381 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="0" t="n">
         <v>115102</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E382" s="0" t="n">
         <v>8.94</v>
@@ -10037,22 +10046,22 @@
         <v>0.08475</v>
       </c>
       <c r="G382" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L382" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="N382" s="5" t="n">
         <f aca="false">AND(E382 &gt; 0, K382 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="0" t="n">
         <v>115103</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E383" s="0" t="n">
         <v>8.44</v>
@@ -10061,31 +10070,31 @@
         <v>0.0863834</v>
       </c>
       <c r="G383" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L383" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="N383" s="5" t="n">
         <f aca="false">AND(E383 &gt; 0, K383 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="0" t="n">
         <v>115104</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E384" s="0" t="n">
         <v>7.9294</v>
       </c>
       <c r="H384" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="L384" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="N384" s="5" t="n">
         <f aca="false">AND(E384 &gt; 0, K384 = "")</f>
@@ -10094,7 +10103,7 @@
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B385" s="0" t="n">
         <v>108401</v>
@@ -10106,10 +10115,10 @@
         <v>2.2</v>
       </c>
       <c r="G385" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L385" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N385" s="5" t="n">
         <f aca="false">AND(E385 &gt; 0, K385 = "")</f>
@@ -10118,7 +10127,7 @@
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B386" s="0" t="n">
         <v>108403</v>
@@ -10130,10 +10139,10 @@
         <v>3.6</v>
       </c>
       <c r="G386" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L386" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N386" s="5" t="n">
         <f aca="false">AND(E386 &gt; 0, K386 = "")</f>
@@ -10142,29 +10151,29 @@
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B387" s="0" t="n">
         <v>108404</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E387" s="6" t="n">
         <v>0.0012</v>
       </c>
       <c r="G387" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L387" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N387" s="5" t="n">
         <f aca="false">AND(E387 &gt; 0, K387 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="0" t="n">
         <v>108408</v>
       </c>
@@ -10175,10 +10184,10 @@
         <v>1</v>
       </c>
       <c r="G388" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L388" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N388" s="5" t="n">
         <f aca="false">AND(E388 &gt; 0, K388 = "")</f>
@@ -10199,10 +10208,10 @@
         <v>7.93</v>
       </c>
       <c r="G389" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L389" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N389" s="5" t="n">
         <f aca="false">AND(E389 &gt; 0, K389 = "")</f>
@@ -10210,7 +10219,36 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:N389"/>
+  <autoFilter ref="A1:N389">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="AlBr"/>
+        <filter val="Alumina"/>
+        <filter val="B4C"/>
+        <filter val="B4C-0.7"/>
+        <filter val="BHC"/>
+        <filter val="Be"/>
+        <filter val="Inconel625"/>
+        <filter val="Inconel718"/>
+        <filter val="LH"/>
+        <filter val="MgO"/>
+        <filter val="NC"/>
+        <filter val="NiAlBr"/>
+        <filter val="OFC"/>
+        <filter val="PZT"/>
+        <filter val="S660"/>
+        <filter val="SS304"/>
+        <filter val="SS304L"/>
+        <filter val="SS316L"/>
+        <filter val="SS316L(N)-IG"/>
+        <filter val="Silica"/>
+        <filter val="W"/>
+        <filter val="XM-19"/>
+        <filter val="air"/>
+        <filter val="water"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fix: restore full default-material-index with merged entries for special indexes for EP11 and UP18
</commit_message>
<xml_diff>
--- a/src/mapstp/data/default-material-index.xlsx
+++ b/src/mapstp/data/default-material-index.xlsx
@@ -12,8 +12,9 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$389</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$N$389</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="545">
   <si>
     <t xml:space="preserve">mnemonic</t>
   </si>
@@ -1297,7 +1298,7 @@
     <t xml:space="preserve">8.2</t>
   </si>
   <si>
-    <t xml:space="preserve">ITER_D_HTN8X3 v2.1</t>
+    <t xml:space="preserve">HTN8X3 v2.1</t>
   </si>
   <si>
     <t xml:space="preserve">WATER</t>
@@ -1550,9 +1551,6 @@
     <t xml:space="preserve">PF1/6 joints, copy of m110805 </t>
   </si>
   <si>
-    <t xml:space="preserve">B4C-0.7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Materials IVVS port and internals</t>
   </si>
   <si>
@@ -1619,6 +1617,9 @@
     <t xml:space="preserve">Mixture of B4C and steel</t>
   </si>
   <si>
+    <t xml:space="preserve">UP18</t>
+  </si>
+  <si>
     <t xml:space="preserve">diamond</t>
   </si>
   <si>
@@ -1668,6 +1669,15 @@
   </si>
   <si>
     <t xml:space="preserve">check density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bot_shield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concrete+5%steel</t>
   </si>
 </sst>
 </file>
@@ -1789,12 +1799,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1804,37 +1814,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N399"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C378" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A378" activeCellId="0" sqref="A378"/>
+      <selection pane="bottomRight" activeCell="C399" activeCellId="0" sqref="C399"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="15.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="15.56"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +1887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
@@ -1905,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>18</v>
       </c>
@@ -1932,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
@@ -1959,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
@@ -1986,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>100</v>
       </c>
@@ -2010,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
         <v>101</v>
       </c>
@@ -2037,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
         <v>102</v>
       </c>
@@ -2067,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>103</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>104</v>
       </c>
@@ -2121,7 +2130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>105</v>
       </c>
@@ -2145,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
         <v>106</v>
       </c>
@@ -2172,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>36</v>
       </c>
@@ -2202,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
         <v>108</v>
       </c>
@@ -2229,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
         <v>109</v>
       </c>
@@ -2253,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
         <v>110</v>
       </c>
@@ -2277,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>43</v>
       </c>
@@ -2304,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <v>112</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>113</v>
       </c>
@@ -2358,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
         <v>120</v>
       </c>
@@ -2391,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
         <v>121</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
         <v>122</v>
       </c>
@@ -2463,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
         <v>123</v>
       </c>
@@ -2490,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
         <v>124</v>
       </c>
@@ -2517,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
         <v>125</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
         <v>190</v>
       </c>
@@ -2571,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
         <v>200</v>
       </c>
@@ -2601,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
         <v>201</v>
       </c>
@@ -2628,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
         <v>202</v>
       </c>
@@ -2661,7 +2670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>71</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>74</v>
       </c>
@@ -2715,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
         <v>250</v>
       </c>
@@ -2739,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
         <v>251</v>
       </c>
@@ -2763,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="n">
         <v>252</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="n">
         <v>253</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="n">
         <v>254</v>
       </c>
@@ -2835,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>83</v>
       </c>
@@ -2865,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="n">
         <v>301</v>
       </c>
@@ -2892,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="n">
         <v>302</v>
       </c>
@@ -2916,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
         <v>303</v>
       </c>
@@ -2943,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>92</v>
       </c>
@@ -2973,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>95</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="n">
         <v>306</v>
       </c>
@@ -3027,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="n">
         <v>350</v>
       </c>
@@ -3051,10 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>103</v>
-      </c>
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="n">
         <v>400</v>
       </c>
@@ -3078,7 +3084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="n">
         <v>906</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="n">
         <v>907</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="n">
         <v>999</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
         <v>9126</v>
       </c>
@@ -3168,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="n">
         <v>97001</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="n">
         <v>107000</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="n">
         <v>150</v>
       </c>
@@ -3240,13 +3246,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="n">
         <v>151</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>115</v>
       </c>
+      <c r="F53" s="0"/>
       <c r="H53" s="0" t="s">
         <v>116</v>
       </c>
@@ -3261,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="n">
         <v>152</v>
       </c>
@@ -3285,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="n">
         <v>153</v>
       </c>
@@ -3303,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="n">
         <v>351</v>
       </c>
@@ -3324,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
         <v>352</v>
       </c>
@@ -3342,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="n">
         <v>353</v>
       </c>
@@ -3360,7 +3367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="n">
         <v>354</v>
       </c>
@@ -3378,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="n">
         <v>355</v>
       </c>
@@ -3396,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="n">
         <v>356</v>
       </c>
@@ -3414,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="n">
         <v>357</v>
       </c>
@@ -3438,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="n">
         <v>358</v>
       </c>
@@ -3462,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="n">
         <v>359</v>
       </c>
@@ -3486,7 +3493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="n">
         <v>360</v>
       </c>
@@ -3504,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="n">
         <v>361</v>
       </c>
@@ -3528,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="n">
         <v>362</v>
       </c>
@@ -3552,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="n">
         <v>363</v>
       </c>
@@ -3576,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="n">
         <v>370</v>
       </c>
@@ -3597,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="n">
         <v>371</v>
       </c>
@@ -3618,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="n">
         <v>372</v>
       </c>
@@ -3639,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="n">
         <v>373</v>
       </c>
@@ -3660,7 +3667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="n">
         <v>374</v>
       </c>
@@ -3681,7 +3688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="n">
         <v>375</v>
       </c>
@@ -3699,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="n">
         <v>376</v>
       </c>
@@ -3717,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="n">
         <v>377</v>
       </c>
@@ -3732,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="n">
         <v>378</v>
       </c>
@@ -3753,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="n">
         <v>379</v>
       </c>
@@ -3774,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="n">
         <v>392</v>
       </c>
@@ -3795,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="n">
         <v>501</v>
       </c>
@@ -3819,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="n">
         <v>521</v>
       </c>
@@ -3843,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="n">
         <v>541</v>
       </c>
@@ -3867,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="n">
         <v>581</v>
       </c>
@@ -3891,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="n">
         <v>2501</v>
       </c>
@@ -3915,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="n">
         <v>2521</v>
       </c>
@@ -3939,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="n">
         <v>2541</v>
       </c>
@@ -3963,7 +3970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="n">
         <v>2581</v>
       </c>
@@ -3987,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="n">
         <v>4501</v>
       </c>
@@ -4011,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="n">
         <v>4521</v>
       </c>
@@ -4035,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="n">
         <v>4541</v>
       </c>
@@ -4059,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="n">
         <v>4581</v>
       </c>
@@ -4083,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="n">
         <v>502</v>
       </c>
@@ -4107,7 +4114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="n">
         <v>522</v>
       </c>
@@ -4131,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="n">
         <v>542</v>
       </c>
@@ -4155,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="n">
         <v>582</v>
       </c>
@@ -4179,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="n">
         <v>2502</v>
       </c>
@@ -4203,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="n">
         <v>2522</v>
       </c>
@@ -4227,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="n">
         <v>2542</v>
       </c>
@@ -4251,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="n">
         <v>2582</v>
       </c>
@@ -4275,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="n">
         <v>4502</v>
       </c>
@@ -4299,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="n">
         <v>4522</v>
       </c>
@@ -4323,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="n">
         <v>4542</v>
       </c>
@@ -4347,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="n">
         <v>4582</v>
       </c>
@@ -4371,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="n">
         <v>503</v>
       </c>
@@ -4395,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="n">
         <v>523</v>
       </c>
@@ -4419,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="n">
         <v>543</v>
       </c>
@@ -4443,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="n">
         <v>583</v>
       </c>
@@ -4467,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="n">
         <v>2503</v>
       </c>
@@ -4491,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="n">
         <v>2523</v>
       </c>
@@ -4515,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="n">
         <v>2543</v>
       </c>
@@ -4539,7 +4546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="n">
         <v>2583</v>
       </c>
@@ -4563,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="n">
         <v>4503</v>
       </c>
@@ -4587,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="n">
         <v>4523</v>
       </c>
@@ -4611,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="n">
         <v>4543</v>
       </c>
@@ -4635,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="n">
         <v>4583</v>
       </c>
@@ -4659,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="6" t="n">
         <v>504</v>
       </c>
@@ -4683,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="6" t="n">
         <v>524</v>
       </c>
@@ -4707,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="6" t="n">
         <v>544</v>
       </c>
@@ -4731,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="6" t="n">
         <v>584</v>
       </c>
@@ -4755,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="n">
         <v>2504</v>
       </c>
@@ -4779,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="n">
         <v>2524</v>
       </c>
@@ -4803,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="n">
         <v>2544</v>
       </c>
@@ -4827,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="n">
         <v>2584</v>
       </c>
@@ -4851,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="n">
         <v>4504</v>
       </c>
@@ -4875,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="n">
         <v>4524</v>
       </c>
@@ -4899,7 +4906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="n">
         <v>4544</v>
       </c>
@@ -4923,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="n">
         <v>4584</v>
       </c>
@@ -4947,7 +4954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="6" t="n">
         <v>505</v>
       </c>
@@ -4971,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="6" t="n">
         <v>525</v>
       </c>
@@ -4995,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="6" t="n">
         <v>545</v>
       </c>
@@ -5019,7 +5026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="6" t="n">
         <v>585</v>
       </c>
@@ -5043,7 +5050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="n">
         <v>2505</v>
       </c>
@@ -5067,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="n">
         <v>2525</v>
       </c>
@@ -5091,7 +5098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="n">
         <v>2545</v>
       </c>
@@ -5115,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="n">
         <v>2585</v>
       </c>
@@ -5139,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="n">
         <v>4505</v>
       </c>
@@ -5163,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="n">
         <v>4525</v>
       </c>
@@ -5187,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="n">
         <v>4545</v>
       </c>
@@ -5211,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="n">
         <v>4585</v>
       </c>
@@ -5235,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="6" t="n">
         <v>506</v>
       </c>
@@ -5259,7 +5266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="6" t="n">
         <v>526</v>
       </c>
@@ -5283,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="6" t="n">
         <v>546</v>
       </c>
@@ -5307,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="6" t="n">
         <v>586</v>
       </c>
@@ -5331,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="n">
         <v>2506</v>
       </c>
@@ -5355,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="n">
         <v>2526</v>
       </c>
@@ -5379,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="n">
         <v>2546</v>
       </c>
@@ -5403,7 +5410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="0" t="n">
         <v>2586</v>
       </c>
@@ -5427,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="0" t="n">
         <v>4506</v>
       </c>
@@ -5451,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="0" t="n">
         <v>4526</v>
       </c>
@@ -5475,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="0" t="n">
         <v>4546</v>
       </c>
@@ -5499,7 +5506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="0" t="n">
         <v>4586</v>
       </c>
@@ -5523,7 +5530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="0" t="n">
         <v>507</v>
       </c>
@@ -5550,7 +5557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="0" t="n">
         <v>527</v>
       </c>
@@ -5577,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="n">
         <v>547</v>
       </c>
@@ -5604,7 +5611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="0" t="n">
         <v>508</v>
       </c>
@@ -5631,7 +5638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="0" t="n">
         <v>528</v>
       </c>
@@ -5658,7 +5665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="0" t="n">
         <v>548</v>
       </c>
@@ -5685,7 +5692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="0" t="n">
         <v>509</v>
       </c>
@@ -5712,7 +5719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="0" t="n">
         <v>529</v>
       </c>
@@ -5739,7 +5746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="0" t="n">
         <v>549</v>
       </c>
@@ -5766,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="0" t="n">
         <v>567</v>
       </c>
@@ -5793,7 +5800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="0" t="n">
         <v>568</v>
       </c>
@@ -5820,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="0" t="n">
         <v>569</v>
       </c>
@@ -5847,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="0" t="n">
         <v>587</v>
       </c>
@@ -5874,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="0" t="n">
         <v>588</v>
       </c>
@@ -5901,7 +5908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="0" t="n">
         <v>589</v>
       </c>
@@ -5928,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="0" t="n">
         <v>2507</v>
       </c>
@@ -5946,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="0" t="n">
         <v>2527</v>
       </c>
@@ -5970,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="0" t="n">
         <v>2547</v>
       </c>
@@ -5994,7 +6001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="0" t="n">
         <v>2508</v>
       </c>
@@ -6018,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="0" t="n">
         <v>2528</v>
       </c>
@@ -6042,7 +6049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="0" t="n">
         <v>2548</v>
       </c>
@@ -6066,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="0" t="n">
         <v>2587</v>
       </c>
@@ -6090,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="0" t="n">
         <v>2588</v>
       </c>
@@ -6114,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="0" t="n">
         <v>2599</v>
       </c>
@@ -6138,7 +6145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="n">
         <v>1510</v>
       </c>
@@ -6168,7 +6175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="0" t="n">
         <v>1530</v>
       </c>
@@ -6198,7 +6205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="0" t="n">
         <v>1550</v>
       </c>
@@ -6228,7 +6235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="0" t="n">
         <v>1590</v>
       </c>
@@ -6258,7 +6265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="0" t="n">
         <v>3511</v>
       </c>
@@ -6288,7 +6295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="0" t="n">
         <v>3531</v>
       </c>
@@ -6318,7 +6325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="0" t="n">
         <v>3551</v>
       </c>
@@ -6348,7 +6355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="0" t="n">
         <v>3591</v>
       </c>
@@ -6378,7 +6385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="0" t="n">
         <v>2511</v>
       </c>
@@ -6408,7 +6415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="0" t="n">
         <v>2531</v>
       </c>
@@ -6438,7 +6445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="n">
         <v>2551</v>
       </c>
@@ -6468,7 +6475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="n">
         <v>2591</v>
       </c>
@@ -6498,7 +6505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="n">
         <v>1511</v>
       </c>
@@ -6522,7 +6529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="0" t="n">
         <v>1531</v>
       </c>
@@ -6546,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="0" t="n">
         <v>1551</v>
       </c>
@@ -6570,7 +6577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="0" t="n">
         <v>1591</v>
       </c>
@@ -6594,7 +6601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="0" t="n">
         <v>511</v>
       </c>
@@ -6618,7 +6625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="0" t="n">
         <v>531</v>
       </c>
@@ -6642,7 +6649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="0" t="n">
         <v>551</v>
       </c>
@@ -6666,7 +6673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="0" t="n">
         <v>591</v>
       </c>
@@ -6690,7 +6697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="0" t="n">
         <v>572</v>
       </c>
@@ -6714,7 +6721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="0" t="n">
         <v>592</v>
       </c>
@@ -6738,7 +6745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="0" t="n">
         <v>512</v>
       </c>
@@ -6762,7 +6769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="0" t="n">
         <v>532</v>
       </c>
@@ -6786,7 +6793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="0" t="n">
         <v>552</v>
       </c>
@@ -6810,7 +6817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="n">
         <v>3592</v>
       </c>
@@ -6834,7 +6841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="0" t="n">
         <v>2592</v>
       </c>
@@ -6858,7 +6865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="0" t="n">
         <v>1592</v>
       </c>
@@ -6882,7 +6889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="0" t="n">
         <v>4513</v>
       </c>
@@ -6897,7 +6904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="0" t="n">
         <v>4533</v>
       </c>
@@ -6912,7 +6919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="0" t="n">
         <v>4553</v>
       </c>
@@ -6927,7 +6934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="n">
         <v>4593</v>
       </c>
@@ -6942,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="0" t="n">
         <v>3513</v>
       </c>
@@ -6957,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="n">
         <v>3533</v>
       </c>
@@ -6972,7 +6979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="0" t="n">
         <v>3553</v>
       </c>
@@ -6987,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="0" t="n">
         <v>3593</v>
       </c>
@@ -7002,7 +7009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="n">
         <v>2513</v>
       </c>
@@ -7017,7 +7024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="0" t="n">
         <v>2533</v>
       </c>
@@ -7032,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="0" t="n">
         <v>2553</v>
       </c>
@@ -7047,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="0" t="n">
         <v>2593</v>
       </c>
@@ -7062,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="n">
         <v>1513</v>
       </c>
@@ -7077,7 +7084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="0" t="n">
         <v>1533</v>
       </c>
@@ -7092,7 +7099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="0" t="n">
         <v>1553</v>
       </c>
@@ -7107,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="n">
         <v>1593</v>
       </c>
@@ -7122,7 +7129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="n">
         <v>513</v>
       </c>
@@ -7137,7 +7144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="0" t="n">
         <v>533</v>
       </c>
@@ -7152,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="n">
         <v>553</v>
       </c>
@@ -7167,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="n">
         <v>593</v>
       </c>
@@ -7182,7 +7189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="n">
         <v>3514</v>
       </c>
@@ -7197,7 +7204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="n">
         <v>3534</v>
       </c>
@@ -7212,7 +7219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="n">
         <v>3554</v>
       </c>
@@ -7227,7 +7234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="n">
         <v>3594</v>
       </c>
@@ -7242,7 +7249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="n">
         <v>1514</v>
       </c>
@@ -7257,7 +7264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="0" t="n">
         <v>1534</v>
       </c>
@@ -7272,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="n">
         <v>1554</v>
       </c>
@@ -7287,7 +7294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="n">
         <v>1594</v>
       </c>
@@ -7302,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="n">
         <v>3515</v>
       </c>
@@ -7317,7 +7324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="n">
         <v>3535</v>
       </c>
@@ -7332,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="n">
         <v>3555</v>
       </c>
@@ -7347,7 +7354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="n">
         <v>3595</v>
       </c>
@@ -7362,7 +7369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="n">
         <v>1515</v>
       </c>
@@ -7377,7 +7384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="n">
         <v>1535</v>
       </c>
@@ -7392,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="n">
         <v>1555</v>
       </c>
@@ -7407,7 +7414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="n">
         <v>1595</v>
       </c>
@@ -7422,7 +7429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="0" t="n">
         <v>4516</v>
       </c>
@@ -7437,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="0" t="n">
         <v>4536</v>
       </c>
@@ -7452,7 +7459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="0" t="n">
         <v>4556</v>
       </c>
@@ -7467,7 +7474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="0" t="n">
         <v>4596</v>
       </c>
@@ -7482,7 +7489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="0" t="n">
         <v>3516</v>
       </c>
@@ -7497,7 +7504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="0" t="n">
         <v>3536</v>
       </c>
@@ -7512,7 +7519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="0" t="n">
         <v>3556</v>
       </c>
@@ -7527,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="0" t="n">
         <v>3596</v>
       </c>
@@ -7542,7 +7549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="0" t="n">
         <v>2516</v>
       </c>
@@ -7557,7 +7564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="0" t="n">
         <v>2536</v>
       </c>
@@ -7572,7 +7579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="0" t="n">
         <v>2556</v>
       </c>
@@ -7587,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="0" t="n">
         <v>2596</v>
       </c>
@@ -7602,7 +7609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="0" t="n">
         <v>1516</v>
       </c>
@@ -7617,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="0" t="n">
         <v>1536</v>
       </c>
@@ -7632,7 +7639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="0" t="n">
         <v>1556</v>
       </c>
@@ -7647,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="0" t="n">
         <v>1596</v>
       </c>
@@ -7662,7 +7669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="n">
         <v>516</v>
       </c>
@@ -7677,7 +7684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="0" t="n">
         <v>536</v>
       </c>
@@ -7692,7 +7699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="0" t="n">
         <v>556</v>
       </c>
@@ -7707,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="0" t="n">
         <v>596</v>
       </c>
@@ -7722,7 +7729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="0" t="n">
         <v>4517</v>
       </c>
@@ -7737,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="0" t="n">
         <v>4537</v>
       </c>
@@ -7752,7 +7759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="0" t="n">
         <v>4557</v>
       </c>
@@ -7767,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="0" t="n">
         <v>4597</v>
       </c>
@@ -7782,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="0" t="n">
         <v>3517</v>
       </c>
@@ -7797,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="0" t="n">
         <v>3537</v>
       </c>
@@ -7812,7 +7819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="0" t="n">
         <v>3557</v>
       </c>
@@ -7827,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="0" t="n">
         <v>3597</v>
       </c>
@@ -7842,7 +7849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="0" t="n">
         <v>2517</v>
       </c>
@@ -7857,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="0" t="n">
         <v>2537</v>
       </c>
@@ -7872,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="0" t="n">
         <v>2557</v>
       </c>
@@ -7887,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="0" t="n">
         <v>2597</v>
       </c>
@@ -7902,7 +7909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="0" t="n">
         <v>1517</v>
       </c>
@@ -7917,7 +7924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="0" t="n">
         <v>1537</v>
       </c>
@@ -7932,7 +7939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="0" t="n">
         <v>1557</v>
       </c>
@@ -7947,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="0" t="n">
         <v>1597</v>
       </c>
@@ -7962,7 +7969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="0" t="n">
         <v>517</v>
       </c>
@@ -7977,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="n">
         <v>537</v>
       </c>
@@ -7992,7 +7999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="n">
         <v>557</v>
       </c>
@@ -8007,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="n">
         <v>597</v>
       </c>
@@ -8022,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="n">
         <v>4518</v>
       </c>
@@ -8037,7 +8044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="n">
         <v>4538</v>
       </c>
@@ -8052,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="n">
         <v>4558</v>
       </c>
@@ -8067,7 +8074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="n">
         <v>4598</v>
       </c>
@@ -8082,7 +8089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="n">
         <v>3518</v>
       </c>
@@ -8097,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="n">
         <v>3538</v>
       </c>
@@ -8112,7 +8119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="n">
         <v>3558</v>
       </c>
@@ -8127,7 +8134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="n">
         <v>3598</v>
       </c>
@@ -8142,7 +8149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="n">
         <v>2518</v>
       </c>
@@ -8157,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="n">
         <v>2538</v>
       </c>
@@ -8172,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="n">
         <v>2558</v>
       </c>
@@ -8187,7 +8194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="n">
         <v>2598</v>
       </c>
@@ -8202,7 +8209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="n">
         <v>1518</v>
       </c>
@@ -8217,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="n">
         <v>1538</v>
       </c>
@@ -8232,7 +8239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="n">
         <v>1558</v>
       </c>
@@ -8247,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="n">
         <v>1598</v>
       </c>
@@ -8262,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="n">
         <v>518</v>
       </c>
@@ -8277,7 +8284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="0" t="n">
         <v>538</v>
       </c>
@@ -8292,7 +8299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B298" s="0" t="n">
         <v>558</v>
       </c>
@@ -8307,7 +8314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="0" t="n">
         <v>598</v>
       </c>
@@ -8322,7 +8329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="0" t="n">
         <v>6007</v>
       </c>
@@ -8334,7 +8341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="0" t="n">
         <v>6008</v>
       </c>
@@ -8346,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="n">
         <v>6009</v>
       </c>
@@ -8358,7 +8365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="0" t="n">
         <v>6010</v>
       </c>
@@ -8370,7 +8377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B304" s="0" t="n">
         <v>7003</v>
       </c>
@@ -8382,7 +8389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B305" s="0" t="n">
         <v>7004</v>
       </c>
@@ -8394,7 +8401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="0" t="n">
         <v>7005</v>
       </c>
@@ -8406,7 +8413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="0" t="n">
         <v>107001</v>
       </c>
@@ -8427,7 +8434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="0" t="n">
         <v>107002</v>
       </c>
@@ -8451,7 +8458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
         <v>419</v>
       </c>
@@ -8461,8 +8468,8 @@
       <c r="C309" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="E309" s="0" t="n">
-        <v>8</v>
+      <c r="E309" s="0" t="s">
+        <v>416</v>
       </c>
       <c r="G309" s="0" t="s">
         <v>417</v>
@@ -8478,7 +8485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="0" t="n">
         <v>107004</v>
       </c>
@@ -8496,7 +8503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
         <v>33</v>
       </c>
@@ -8506,8 +8513,8 @@
       <c r="C311" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E311" s="0" t="n">
-        <v>7.93</v>
+      <c r="E311" s="0" t="s">
+        <v>412</v>
       </c>
       <c r="G311" s="0" t="s">
         <v>417</v>
@@ -8520,7 +8527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="0" t="n">
         <v>107006</v>
       </c>
@@ -8541,7 +8548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="0" t="n">
         <v>107007</v>
       </c>
@@ -8559,7 +8566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="n">
         <v>107009</v>
       </c>
@@ -8580,7 +8587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="0" t="n">
         <v>107301</v>
       </c>
@@ -8604,7 +8611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
         <v>24</v>
       </c>
@@ -8614,8 +8621,8 @@
       <c r="C316" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E316" s="0" t="n">
-        <v>7.93</v>
+      <c r="E316" s="0" t="s">
+        <v>412</v>
       </c>
       <c r="G316" s="0" t="s">
         <v>417</v>
@@ -8631,7 +8638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="0" t="n">
         <v>107303</v>
       </c>
@@ -8655,7 +8662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="0" t="n">
         <v>107304</v>
       </c>
@@ -8679,7 +8686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
         <v>429</v>
       </c>
@@ -8689,8 +8696,8 @@
       <c r="C319" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="E319" s="0" t="n">
-        <v>7.6</v>
+      <c r="E319" s="0" t="s">
+        <v>422</v>
       </c>
       <c r="G319" s="0" t="s">
         <v>417</v>
@@ -8703,7 +8710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="0" t="n">
         <v>107306</v>
       </c>
@@ -8724,7 +8731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="n">
         <v>107307</v>
       </c>
@@ -8742,7 +8749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="0" t="n">
         <v>107308</v>
       </c>
@@ -8760,7 +8767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="n">
         <v>107309</v>
       </c>
@@ -8781,7 +8788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="0" t="n">
         <v>107310</v>
       </c>
@@ -8802,7 +8809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="n">
         <v>107311</v>
       </c>
@@ -8817,7 +8824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="0" t="n">
         <v>107701</v>
       </c>
@@ -8841,7 +8848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="n">
         <v>107702</v>
       </c>
@@ -8865,7 +8872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="n">
         <v>107703</v>
       </c>
@@ -8886,7 +8893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="0" t="n">
         <v>108001</v>
       </c>
@@ -8910,7 +8917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="0" t="n">
         <v>108002</v>
       </c>
@@ -8934,7 +8941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="0" t="n">
         <v>108003</v>
       </c>
@@ -8955,7 +8962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B332" s="0" t="n">
         <v>108502</v>
       </c>
@@ -8973,7 +8980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B333" s="0" t="n">
         <v>108511</v>
       </c>
@@ -8994,7 +9001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="0" t="n">
         <v>108512</v>
       </c>
@@ -9015,7 +9022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="0" t="n">
         <v>108513</v>
       </c>
@@ -9036,7 +9043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="0" t="n">
         <v>108514</v>
       </c>
@@ -9057,7 +9064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B337" s="0" t="n">
         <v>108515</v>
       </c>
@@ -9078,7 +9085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B338" s="0" t="n">
         <v>108516</v>
       </c>
@@ -9099,7 +9106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B339" s="0" t="n">
         <v>108517</v>
       </c>
@@ -9120,7 +9127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B340" s="0" t="n">
         <v>108518</v>
       </c>
@@ -9144,7 +9151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B341" s="0" t="n">
         <v>108519</v>
       </c>
@@ -9162,7 +9169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="0" t="n">
         <v>108520</v>
       </c>
@@ -9180,7 +9187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B343" s="0" t="n">
         <v>110501</v>
       </c>
@@ -9201,7 +9208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B344" s="0" t="n">
         <v>110502</v>
       </c>
@@ -9222,7 +9229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B345" s="0" t="n">
         <v>110503</v>
       </c>
@@ -9243,7 +9250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="0" t="n">
         <v>110504</v>
       </c>
@@ -9264,7 +9271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B347" s="0" t="n">
         <v>110505</v>
       </c>
@@ -9282,7 +9289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="0" t="n">
         <v>110506</v>
       </c>
@@ -9300,7 +9307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="112.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="56.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B349" s="0" t="n">
         <v>110507</v>
       </c>
@@ -9327,7 +9334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B350" s="0" t="n">
         <v>110801</v>
       </c>
@@ -9351,7 +9358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="112.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="34.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B351" s="0" t="n">
         <v>110802</v>
       </c>
@@ -9375,7 +9382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B352" s="0" t="n">
         <v>110803</v>
       </c>
@@ -9393,7 +9400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="150" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="67.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="0" t="n">
         <v>110804</v>
       </c>
@@ -9420,7 +9427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="200" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="89.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B354" s="0" t="n">
         <v>110805</v>
       </c>
@@ -9430,7 +9437,7 @@
       <c r="E354" s="0" t="n">
         <v>5.27505</v>
       </c>
-      <c r="F354" s="1" t="n">
+      <c r="F354" s="0" t="n">
         <v>0.0881</v>
       </c>
       <c r="H354" s="8" t="s">
@@ -9447,7 +9454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B355" s="0" t="n">
         <v>110901</v>
       </c>
@@ -9474,7 +9481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B356" s="0" t="n">
         <v>110902</v>
       </c>
@@ -9501,7 +9508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B357" s="0" t="n">
         <v>110903</v>
       </c>
@@ -9528,7 +9535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B358" s="0" t="n">
         <v>111101</v>
       </c>
@@ -9555,7 +9562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="0" t="n">
         <v>111102</v>
       </c>
@@ -9582,7 +9589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B360" s="0" t="n">
         <v>111103</v>
       </c>
@@ -9609,7 +9616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B361" s="0" t="n">
         <v>110851</v>
       </c>
@@ -9627,7 +9634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B362" s="0" t="n">
         <v>110852</v>
       </c>
@@ -9651,7 +9658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="200" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="89.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="0" t="n">
         <v>110853</v>
       </c>
@@ -9678,7 +9685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B364" s="0" t="n">
         <v>110951</v>
       </c>
@@ -9696,7 +9703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B365" s="0" t="n">
         <v>110952</v>
       </c>
@@ -9720,7 +9727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B366" s="0" t="n">
         <v>110953</v>
       </c>
@@ -9747,7 +9754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B367" s="0" t="n">
         <v>111151</v>
       </c>
@@ -9765,7 +9772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="0" t="n">
         <v>111152</v>
       </c>
@@ -9789,7 +9796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="0" t="n">
         <v>111153</v>
       </c>
@@ -9816,7 +9823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="0" t="n">
         <v>111251</v>
       </c>
@@ -9834,7 +9841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="0" t="n">
         <v>111252</v>
       </c>
@@ -9858,7 +9865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="0" t="n">
         <v>111253</v>
       </c>
@@ -9885,7 +9892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="0" t="n">
         <v>111351</v>
       </c>
@@ -9903,7 +9910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" customFormat="false" ht="23.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B374" s="0" t="n">
         <v>111352</v>
       </c>
@@ -9927,7 +9934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" customFormat="false" ht="200" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="89.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B375" s="0" t="n">
         <v>11353</v>
       </c>
@@ -9951,10 +9958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="0" t="s">
-        <v>502</v>
-      </c>
+    <row r="376" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B376" s="0" t="n">
         <v>114101</v>
       </c>
@@ -9971,82 +9975,82 @@
         <v>48</v>
       </c>
       <c r="L376" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N376" s="0" t="n">
         <f aca="false">AND(E376 &gt; 0, K376 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="377" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B377" s="0" t="n">
         <v>114102</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E377" s="0" t="n">
         <v>2.32</v>
       </c>
       <c r="L377" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N377" s="0" t="n">
         <f aca="false">AND(E377 &gt; 0, K377 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="378" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B378" s="0" t="n">
         <v>114103</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E378" s="0" t="n">
         <v>7.7</v>
       </c>
       <c r="L378" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N378" s="0" t="n">
         <f aca="false">AND(E378 &gt; 0, K378 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="379" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B379" s="0" t="n">
         <v>114104</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E379" s="0" t="n">
         <v>3.97</v>
       </c>
       <c r="L379" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N379" s="0" t="n">
         <f aca="false">AND(E379 &gt; 0, K379 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="380" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="0" t="n">
         <v>115100</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E380" s="0" t="n">
         <v>7.93</v>
@@ -10055,22 +10059,22 @@
         <v>0.086353</v>
       </c>
       <c r="G380" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="L380" s="0" t="s">
         <v>508</v>
-      </c>
-      <c r="L380" s="0" t="s">
-        <v>509</v>
       </c>
       <c r="N380" s="0" t="n">
         <f aca="false">AND(E380 &gt; 0, K380 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="0" t="n">
         <v>115101</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E381" s="0" t="n">
         <v>2.7</v>
@@ -10079,22 +10083,22 @@
         <v>0.080544</v>
       </c>
       <c r="G381" s="0" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L381" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="N381" s="0" t="n">
         <f aca="false">AND(E381 &gt; 0, K381 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="382" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="0" t="n">
         <v>115102</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E382" s="0" t="n">
         <v>8.94</v>
@@ -10103,22 +10107,22 @@
         <v>0.08475</v>
       </c>
       <c r="G382" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="L382" s="0" t="s">
         <v>508</v>
-      </c>
-      <c r="L382" s="0" t="s">
-        <v>509</v>
       </c>
       <c r="N382" s="0" t="n">
         <f aca="false">AND(E382 &gt; 0, K382 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="383" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="0" t="n">
         <v>115103</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E383" s="0" t="n">
         <v>8.44</v>
@@ -10127,40 +10131,40 @@
         <v>0.0863834</v>
       </c>
       <c r="G383" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="L383" s="0" t="s">
         <v>508</v>
-      </c>
-      <c r="L383" s="0" t="s">
-        <v>509</v>
       </c>
       <c r="N383" s="0" t="n">
         <f aca="false">AND(E383 &gt; 0, K383 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="384" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="0" t="n">
         <v>115104</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E384" s="0" t="n">
         <v>7.9294</v>
       </c>
       <c r="H384" s="0" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L384" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="N384" s="0" t="n">
         <f aca="false">AND(E384 &gt; 0, K384 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="385" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B385" s="0" t="n">
         <v>108401</v>
@@ -10172,19 +10176,19 @@
         <v>2.2</v>
       </c>
       <c r="G385" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="L385" s="0" t="s">
         <v>517</v>
-      </c>
-      <c r="L385" s="0" t="s">
-        <v>518</v>
       </c>
       <c r="N385" s="0" t="n">
         <f aca="false">AND(E385 &gt; 0, K385 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="386" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B386" s="0" t="n">
         <v>108403</v>
@@ -10196,41 +10200,41 @@
         <v>3.6</v>
       </c>
       <c r="G386" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="L386" s="0" t="s">
         <v>517</v>
-      </c>
-      <c r="L386" s="0" t="s">
-        <v>518</v>
       </c>
       <c r="N386" s="0" t="n">
         <f aca="false">AND(E386 &gt; 0, K386 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="387" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B387" s="0" t="n">
         <v>108404</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E387" s="5" t="n">
         <v>0.0012</v>
       </c>
       <c r="G387" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="L387" s="0" t="s">
         <v>517</v>
-      </c>
-      <c r="L387" s="0" t="s">
-        <v>518</v>
       </c>
       <c r="N387" s="0" t="n">
         <f aca="false">AND(E387 &gt; 0, K387 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="388" customFormat="false" ht="12.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="0" t="n">
         <v>108408</v>
       </c>
@@ -10241,17 +10245,17 @@
         <v>1</v>
       </c>
       <c r="G388" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L388" s="0" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N388" s="0" t="n">
         <f aca="false">AND(E388 &gt; 0, K388 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="389" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
         <v>32</v>
       </c>
@@ -10265,31 +10269,38 @@
         <v>7.93</v>
       </c>
       <c r="G389" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L389" s="0" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N389" s="0" t="n">
         <f aca="false">AND(E389 &gt; 0, K389 = "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="390" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B390" s="0" t="n">
         <v>170000</v>
       </c>
       <c r="C390" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E390" s="0" t="n">
         <v>2.662</v>
       </c>
-    </row>
-    <row r="391" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L390" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N390" s="0" t="n">
+        <f aca="false">AND(E390 &gt; 0, K390 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
         <v>525</v>
       </c>
@@ -10302,8 +10313,15 @@
       <c r="E391" s="0" t="n">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="392" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L391" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N391" s="0" t="n">
+        <f aca="false">AND(E391 &gt; 0, K391 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
         <v>527</v>
       </c>
@@ -10316,8 +10334,15 @@
       <c r="E392" s="9" t="n">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="393" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L392" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N392" s="0" t="n">
+        <f aca="false">AND(E392 &gt; 0, K392 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
         <v>529</v>
       </c>
@@ -10330,8 +10355,15 @@
       <c r="E393" s="9" t="n">
         <v>7.93</v>
       </c>
-    </row>
-    <row r="394" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L393" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N393" s="0" t="n">
+        <f aca="false">AND(E393 &gt; 0, K393 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
         <v>531</v>
       </c>
@@ -10344,8 +10376,15 @@
       <c r="E394" s="9" t="n">
         <v>8.92</v>
       </c>
-    </row>
-    <row r="395" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L394" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N394" s="0" t="n">
+        <f aca="false">AND(E394 &gt; 0, K394 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
         <v>533</v>
       </c>
@@ -10358,8 +10397,15 @@
       <c r="E395" s="9" t="n">
         <v>1.636</v>
       </c>
-    </row>
-    <row r="396" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L395" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N395" s="0" t="n">
+        <f aca="false">AND(E395 &gt; 0, K395 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
         <v>535</v>
       </c>
@@ -10372,8 +10418,15 @@
       <c r="E396" s="9" t="n">
         <v>1.801</v>
       </c>
-    </row>
-    <row r="397" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L396" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N396" s="0" t="n">
+        <f aca="false">AND(E396 &gt; 0, K396 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
         <v>537</v>
       </c>
@@ -10386,8 +10439,15 @@
       <c r="E397" s="9" t="n">
         <v>5.19</v>
       </c>
-    </row>
-    <row r="398" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L397" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N397" s="0" t="n">
+        <f aca="false">AND(E397 &gt; 0, K397 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
         <v>539</v>
       </c>
@@ -10403,10 +10463,60 @@
       <c r="H398" s="0" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="L398" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="N398" s="0" t="n">
+        <f aca="false">AND(E398 &gt; 0, K398 = "")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="B399" s="0" t="n">
+        <v>170010</v>
+      </c>
+      <c r="C399" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="E399" s="9" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="L399" s="0" t="s">
+        <v>542</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N389"/>
+  <autoFilter ref="A1:N389">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="AlBr"/>
+        <filter val="Alumina"/>
+        <filter val="B4C"/>
+        <filter val="BHC"/>
+        <filter val="Be"/>
+        <filter val="Inconel625"/>
+        <filter val="Inconel718"/>
+        <filter val="LH"/>
+        <filter val="MgO"/>
+        <filter val="NC"/>
+        <filter val="NiAlBr"/>
+        <filter val="OFC"/>
+        <filter val="PZT"/>
+        <filter val="S660"/>
+        <filter val="SS304"/>
+        <filter val="SS304L"/>
+        <filter val="SS316L"/>
+        <filter val="SS316L(N)-IG"/>
+        <filter val="SXM"/>
+        <filter val="Silica"/>
+        <filter val="W"/>
+        <filter val="air"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
build: update default material index with ep11 data
</commit_message>
<xml_diff>
--- a/src/mapstp/data/default-material-index.xlsx
+++ b/src/mapstp/data/default-material-index.xlsx
@@ -11,8 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$399</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$N$389</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$389</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="563">
   <si>
     <t xml:space="preserve">mnemonic</t>
   </si>
@@ -1620,9 +1619,6 @@
     <t xml:space="preserve">Mixture of B4C and steel</t>
   </si>
   <si>
-    <t xml:space="preserve">EP11, UP18</t>
-  </si>
-  <si>
     <t xml:space="preserve">diamond</t>
   </si>
   <si>
@@ -1678,6 +1674,63 @@
   </si>
   <si>
     <t xml:space="preserve">Concrete+5%steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPGe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G-75%; Fe-10%; Ni-3%; Cr-2% ; Al-10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-2%, Mn-20%, P-1.5%, S-1.5%, N-1%, Cu-6%, Sn-1%, Fe-%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stilbene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14H12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LiH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H=50%; 6Li=3.75%; 7Li=46.25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS304B4C(7030)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS304(70%)+B4C(30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlB4C(3664)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al(36%)+B4C(64%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SiO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LaBr3Ce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lanthan Bromide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La=34.3 Br=59.7 Ce=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%wgt</t>
   </si>
 </sst>
 </file>
@@ -1799,36 +1852,40 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N408"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B379" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B376" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A379" activeCellId="0" sqref="A379"/>
-      <selection pane="bottomRight" activeCell="A380" activeCellId="0" sqref="A380"/>
+      <selection pane="bottomLeft" activeCell="A376" activeCellId="0" sqref="A376"/>
+      <selection pane="bottomRight" activeCell="A404" activeCellId="0" sqref="A404"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="93.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.43"/>
@@ -1837,6 +1894,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>100</v>
       </c>
@@ -2015,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
         <v>101</v>
       </c>
@@ -2042,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
         <v>102</v>
       </c>
@@ -2072,7 +2130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>103</v>
       </c>
@@ -2102,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>104</v>
       </c>
@@ -2126,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>105</v>
       </c>
@@ -2150,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
         <v>106</v>
       </c>
@@ -2207,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
         <v>108</v>
       </c>
@@ -2234,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
         <v>109</v>
       </c>
@@ -2258,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
         <v>110</v>
       </c>
@@ -2309,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <v>112</v>
       </c>
@@ -2336,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>113</v>
       </c>
@@ -2363,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
         <v>120</v>
       </c>
@@ -2396,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
         <v>121</v>
       </c>
@@ -2432,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
         <v>122</v>
       </c>
@@ -2468,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
         <v>123</v>
       </c>
@@ -2495,7 +2553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
         <v>124</v>
       </c>
@@ -2522,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
         <v>125</v>
       </c>
@@ -2546,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
         <v>190</v>
       </c>
@@ -2576,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
         <v>200</v>
       </c>
@@ -2606,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
         <v>201</v>
       </c>
@@ -2633,7 +2691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
         <v>202</v>
       </c>
@@ -2720,7 +2778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
         <v>250</v>
       </c>
@@ -2744,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
         <v>251</v>
       </c>
@@ -2768,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="n">
         <v>252</v>
       </c>
@@ -2792,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="n">
         <v>253</v>
       </c>
@@ -2816,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="n">
         <v>254</v>
       </c>
@@ -2870,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="n">
         <v>301</v>
       </c>
@@ -2897,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="n">
         <v>302</v>
       </c>
@@ -2921,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
         <v>303</v>
       </c>
@@ -3005,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="n">
         <v>306</v>
       </c>
@@ -3032,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="n">
         <v>350</v>
       </c>
@@ -3083,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="n">
         <v>906</v>
       </c>
@@ -3107,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="n">
         <v>907</v>
       </c>
@@ -3128,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="n">
         <v>999</v>
       </c>
@@ -3149,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
         <v>9126</v>
       </c>
@@ -3173,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="n">
         <v>97001</v>
       </c>
@@ -3200,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="n">
         <v>107000</v>
       </c>
@@ -3227,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="n">
         <v>150</v>
       </c>
@@ -3245,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="n">
         <v>151</v>
       </c>
@@ -3266,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="n">
         <v>152</v>
       </c>
@@ -3290,7 +3348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="n">
         <v>153</v>
       </c>
@@ -3308,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="n">
         <v>351</v>
       </c>
@@ -3329,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
         <v>352</v>
       </c>
@@ -3347,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="n">
         <v>353</v>
       </c>
@@ -3365,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="n">
         <v>354</v>
       </c>
@@ -3383,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="n">
         <v>355</v>
       </c>
@@ -3401,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="n">
         <v>356</v>
       </c>
@@ -3419,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="n">
         <v>357</v>
       </c>
@@ -3443,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="n">
         <v>358</v>
       </c>
@@ -3467,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="n">
         <v>359</v>
       </c>
@@ -3491,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="n">
         <v>360</v>
       </c>
@@ -3509,7 +3567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="n">
         <v>361</v>
       </c>
@@ -3533,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="n">
         <v>362</v>
       </c>
@@ -3557,7 +3615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="n">
         <v>363</v>
       </c>
@@ -3581,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="n">
         <v>370</v>
       </c>
@@ -3602,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="n">
         <v>371</v>
       </c>
@@ -3623,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="n">
         <v>372</v>
       </c>
@@ -3644,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="n">
         <v>373</v>
       </c>
@@ -3665,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="n">
         <v>374</v>
       </c>
@@ -3686,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="n">
         <v>375</v>
       </c>
@@ -3704,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="n">
         <v>376</v>
       </c>
@@ -3722,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="n">
         <v>377</v>
       </c>
@@ -3737,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="n">
         <v>378</v>
       </c>
@@ -3758,7 +3816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="n">
         <v>379</v>
       </c>
@@ -3779,7 +3837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="n">
         <v>392</v>
       </c>
@@ -3800,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="n">
         <v>501</v>
       </c>
@@ -3824,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="n">
         <v>521</v>
       </c>
@@ -3848,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="n">
         <v>541</v>
       </c>
@@ -3872,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="n">
         <v>581</v>
       </c>
@@ -3896,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="n">
         <v>2501</v>
       </c>
@@ -3920,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="n">
         <v>2521</v>
       </c>
@@ -3944,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="n">
         <v>2541</v>
       </c>
@@ -3968,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="n">
         <v>2581</v>
       </c>
@@ -3992,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="n">
         <v>4501</v>
       </c>
@@ -4016,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="n">
         <v>4521</v>
       </c>
@@ -4040,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="n">
         <v>4541</v>
       </c>
@@ -4064,7 +4122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="n">
         <v>4581</v>
       </c>
@@ -4088,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="n">
         <v>502</v>
       </c>
@@ -4112,7 +4170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="n">
         <v>522</v>
       </c>
@@ -4136,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="n">
         <v>542</v>
       </c>
@@ -4160,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="n">
         <v>582</v>
       </c>
@@ -4184,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="n">
         <v>2502</v>
       </c>
@@ -4208,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="n">
         <v>2522</v>
       </c>
@@ -4232,7 +4290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="n">
         <v>2542</v>
       </c>
@@ -4256,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="n">
         <v>2582</v>
       </c>
@@ -4280,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="n">
         <v>4502</v>
       </c>
@@ -4304,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="n">
         <v>4522</v>
       </c>
@@ -4328,7 +4386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="n">
         <v>4542</v>
       </c>
@@ -4352,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="n">
         <v>4582</v>
       </c>
@@ -4376,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="n">
         <v>503</v>
       </c>
@@ -4400,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="n">
         <v>523</v>
       </c>
@@ -4424,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="n">
         <v>543</v>
       </c>
@@ -4448,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="n">
         <v>583</v>
       </c>
@@ -4472,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="n">
         <v>2503</v>
       </c>
@@ -4496,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="n">
         <v>2523</v>
       </c>
@@ -4520,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="n">
         <v>2543</v>
       </c>
@@ -4544,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="n">
         <v>2583</v>
       </c>
@@ -4568,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="n">
         <v>4503</v>
       </c>
@@ -4592,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="n">
         <v>4523</v>
       </c>
@@ -4616,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="n">
         <v>4543</v>
       </c>
@@ -4640,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="n">
         <v>4583</v>
       </c>
@@ -4664,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="6" t="n">
         <v>504</v>
       </c>
@@ -4688,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="6" t="n">
         <v>524</v>
       </c>
@@ -4712,7 +4770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="6" t="n">
         <v>544</v>
       </c>
@@ -4736,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="6" t="n">
         <v>584</v>
       </c>
@@ -4760,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="n">
         <v>2504</v>
       </c>
@@ -4784,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="n">
         <v>2524</v>
       </c>
@@ -4808,7 +4866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="n">
         <v>2544</v>
       </c>
@@ -4832,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="n">
         <v>2584</v>
       </c>
@@ -4856,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="n">
         <v>4504</v>
       </c>
@@ -4880,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="n">
         <v>4524</v>
       </c>
@@ -4904,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="n">
         <v>4544</v>
       </c>
@@ -4928,7 +4986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="n">
         <v>4584</v>
       </c>
@@ -4952,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="6" t="n">
         <v>505</v>
       </c>
@@ -4976,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="6" t="n">
         <v>525</v>
       </c>
@@ -5000,7 +5058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="6" t="n">
         <v>545</v>
       </c>
@@ -5024,7 +5082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="6" t="n">
         <v>585</v>
       </c>
@@ -5048,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="0" t="n">
         <v>2505</v>
       </c>
@@ -5072,7 +5130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="n">
         <v>2525</v>
       </c>
@@ -5096,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="n">
         <v>2545</v>
       </c>
@@ -5120,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="n">
         <v>2585</v>
       </c>
@@ -5144,7 +5202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="0" t="n">
         <v>4505</v>
       </c>
@@ -5168,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="0" t="n">
         <v>4525</v>
       </c>
@@ -5192,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="n">
         <v>4545</v>
       </c>
@@ -5216,7 +5274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="n">
         <v>4585</v>
       </c>
@@ -5240,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="6" t="n">
         <v>506</v>
       </c>
@@ -5264,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="6" t="n">
         <v>526</v>
       </c>
@@ -5288,7 +5346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="6" t="n">
         <v>546</v>
       </c>
@@ -5312,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="6" t="n">
         <v>586</v>
       </c>
@@ -5336,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="n">
         <v>2506</v>
       </c>
@@ -5360,7 +5418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="n">
         <v>2526</v>
       </c>
@@ -5384,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="n">
         <v>2546</v>
       </c>
@@ -5408,7 +5466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="0" t="n">
         <v>2586</v>
       </c>
@@ -5432,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="0" t="n">
         <v>4506</v>
       </c>
@@ -5456,7 +5514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="0" t="n">
         <v>4526</v>
       </c>
@@ -5480,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="0" t="n">
         <v>4546</v>
       </c>
@@ -5504,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="0" t="n">
         <v>4586</v>
       </c>
@@ -5528,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="0" t="n">
         <v>507</v>
       </c>
@@ -5555,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="0" t="n">
         <v>527</v>
       </c>
@@ -5582,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="n">
         <v>547</v>
       </c>
@@ -5609,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="0" t="n">
         <v>508</v>
       </c>
@@ -5636,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="0" t="n">
         <v>528</v>
       </c>
@@ -5663,7 +5721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="0" t="n">
         <v>548</v>
       </c>
@@ -5690,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="0" t="n">
         <v>509</v>
       </c>
@@ -5717,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="0" t="n">
         <v>529</v>
       </c>
@@ -5744,7 +5802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="0" t="n">
         <v>549</v>
       </c>
@@ -5771,7 +5829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="0" t="n">
         <v>567</v>
       </c>
@@ -5798,7 +5856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="0" t="n">
         <v>568</v>
       </c>
@@ -5825,7 +5883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="0" t="n">
         <v>569</v>
       </c>
@@ -5852,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="0" t="n">
         <v>587</v>
       </c>
@@ -5879,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="0" t="n">
         <v>588</v>
       </c>
@@ -5906,7 +5964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="0" t="n">
         <v>589</v>
       </c>
@@ -5933,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="0" t="n">
         <v>2507</v>
       </c>
@@ -5951,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="0" t="n">
         <v>2527</v>
       </c>
@@ -5975,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="0" t="n">
         <v>2547</v>
       </c>
@@ -5999,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="0" t="n">
         <v>2508</v>
       </c>
@@ -6023,7 +6081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="0" t="n">
         <v>2528</v>
       </c>
@@ -6047,7 +6105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="0" t="n">
         <v>2548</v>
       </c>
@@ -6071,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="0" t="n">
         <v>2587</v>
       </c>
@@ -6095,7 +6153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="0" t="n">
         <v>2588</v>
       </c>
@@ -6119,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="0" t="n">
         <v>2599</v>
       </c>
@@ -6143,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="n">
         <v>1510</v>
       </c>
@@ -6173,7 +6231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="0" t="n">
         <v>1530</v>
       </c>
@@ -6203,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="0" t="n">
         <v>1550</v>
       </c>
@@ -6233,7 +6291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="0" t="n">
         <v>1590</v>
       </c>
@@ -6263,7 +6321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="0" t="n">
         <v>3511</v>
       </c>
@@ -6293,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="0" t="n">
         <v>3531</v>
       </c>
@@ -6323,7 +6381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="0" t="n">
         <v>3551</v>
       </c>
@@ -6353,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="0" t="n">
         <v>3591</v>
       </c>
@@ -6383,7 +6441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="0" t="n">
         <v>2511</v>
       </c>
@@ -6413,7 +6471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="0" t="n">
         <v>2531</v>
       </c>
@@ -6443,7 +6501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="n">
         <v>2551</v>
       </c>
@@ -6473,7 +6531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="n">
         <v>2591</v>
       </c>
@@ -6503,7 +6561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="n">
         <v>1511</v>
       </c>
@@ -6527,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="0" t="n">
         <v>1531</v>
       </c>
@@ -6551,7 +6609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="0" t="n">
         <v>1551</v>
       </c>
@@ -6575,7 +6633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="0" t="n">
         <v>1591</v>
       </c>
@@ -6599,7 +6657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="0" t="n">
         <v>511</v>
       </c>
@@ -6623,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="0" t="n">
         <v>531</v>
       </c>
@@ -6647,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="0" t="n">
         <v>551</v>
       </c>
@@ -6671,7 +6729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="0" t="n">
         <v>591</v>
       </c>
@@ -6695,7 +6753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="0" t="n">
         <v>572</v>
       </c>
@@ -6719,7 +6777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="0" t="n">
         <v>592</v>
       </c>
@@ -6743,7 +6801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="0" t="n">
         <v>512</v>
       </c>
@@ -6767,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="0" t="n">
         <v>532</v>
       </c>
@@ -6791,7 +6849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="0" t="n">
         <v>552</v>
       </c>
@@ -6815,7 +6873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="n">
         <v>3592</v>
       </c>
@@ -6839,7 +6897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="0" t="n">
         <v>2592</v>
       </c>
@@ -6863,7 +6921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="0" t="n">
         <v>1592</v>
       </c>
@@ -6887,7 +6945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="0" t="n">
         <v>4513</v>
       </c>
@@ -6902,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="0" t="n">
         <v>4533</v>
       </c>
@@ -6917,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="0" t="n">
         <v>4553</v>
       </c>
@@ -6932,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="n">
         <v>4593</v>
       </c>
@@ -6947,7 +7005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="0" t="n">
         <v>3513</v>
       </c>
@@ -6962,7 +7020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="n">
         <v>3533</v>
       </c>
@@ -6977,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="0" t="n">
         <v>3553</v>
       </c>
@@ -6992,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="0" t="n">
         <v>3593</v>
       </c>
@@ -7007,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="n">
         <v>2513</v>
       </c>
@@ -7022,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="0" t="n">
         <v>2533</v>
       </c>
@@ -7037,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="0" t="n">
         <v>2553</v>
       </c>
@@ -7052,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="0" t="n">
         <v>2593</v>
       </c>
@@ -7067,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="n">
         <v>1513</v>
       </c>
@@ -7082,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="0" t="n">
         <v>1533</v>
       </c>
@@ -7097,7 +7155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="0" t="n">
         <v>1553</v>
       </c>
@@ -7112,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="n">
         <v>1593</v>
       </c>
@@ -7127,7 +7185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="n">
         <v>513</v>
       </c>
@@ -7142,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="0" t="n">
         <v>533</v>
       </c>
@@ -7157,7 +7215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="n">
         <v>553</v>
       </c>
@@ -7172,7 +7230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="n">
         <v>593</v>
       </c>
@@ -7187,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="n">
         <v>3514</v>
       </c>
@@ -7202,7 +7260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="n">
         <v>3534</v>
       </c>
@@ -7217,7 +7275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="n">
         <v>3554</v>
       </c>
@@ -7232,7 +7290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="n">
         <v>3594</v>
       </c>
@@ -7247,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="n">
         <v>1514</v>
       </c>
@@ -7262,7 +7320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="0" t="n">
         <v>1534</v>
       </c>
@@ -7277,7 +7335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="n">
         <v>1554</v>
       </c>
@@ -7292,7 +7350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="n">
         <v>1594</v>
       </c>
@@ -7307,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="n">
         <v>3515</v>
       </c>
@@ -7322,7 +7380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="n">
         <v>3535</v>
       </c>
@@ -7337,7 +7395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="n">
         <v>3555</v>
       </c>
@@ -7352,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="n">
         <v>3595</v>
       </c>
@@ -7367,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="n">
         <v>1515</v>
       </c>
@@ -7382,7 +7440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="n">
         <v>1535</v>
       </c>
@@ -7397,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="n">
         <v>1555</v>
       </c>
@@ -7412,7 +7470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="n">
         <v>1595</v>
       </c>
@@ -7427,7 +7485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="0" t="n">
         <v>4516</v>
       </c>
@@ -7442,7 +7500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="0" t="n">
         <v>4536</v>
       </c>
@@ -7457,7 +7515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="0" t="n">
         <v>4556</v>
       </c>
@@ -7472,7 +7530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="0" t="n">
         <v>4596</v>
       </c>
@@ -7487,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="0" t="n">
         <v>3516</v>
       </c>
@@ -7502,7 +7560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="0" t="n">
         <v>3536</v>
       </c>
@@ -7517,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="0" t="n">
         <v>3556</v>
       </c>
@@ -7532,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="0" t="n">
         <v>3596</v>
       </c>
@@ -7547,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="0" t="n">
         <v>2516</v>
       </c>
@@ -7562,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="0" t="n">
         <v>2536</v>
       </c>
@@ -7577,7 +7635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="0" t="n">
         <v>2556</v>
       </c>
@@ -7592,7 +7650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="0" t="n">
         <v>2596</v>
       </c>
@@ -7607,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="0" t="n">
         <v>1516</v>
       </c>
@@ -7622,7 +7680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="0" t="n">
         <v>1536</v>
       </c>
@@ -7637,7 +7695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="0" t="n">
         <v>1556</v>
       </c>
@@ -7652,7 +7710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="0" t="n">
         <v>1596</v>
       </c>
@@ -7667,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="n">
         <v>516</v>
       </c>
@@ -7682,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="0" t="n">
         <v>536</v>
       </c>
@@ -7697,7 +7755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="0" t="n">
         <v>556</v>
       </c>
@@ -7712,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="0" t="n">
         <v>596</v>
       </c>
@@ -7727,7 +7785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="0" t="n">
         <v>4517</v>
       </c>
@@ -7742,7 +7800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="0" t="n">
         <v>4537</v>
       </c>
@@ -7757,7 +7815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="0" t="n">
         <v>4557</v>
       </c>
@@ -7772,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="0" t="n">
         <v>4597</v>
       </c>
@@ -7787,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="0" t="n">
         <v>3517</v>
       </c>
@@ -7802,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="0" t="n">
         <v>3537</v>
       </c>
@@ -7817,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="0" t="n">
         <v>3557</v>
       </c>
@@ -7832,7 +7890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="0" t="n">
         <v>3597</v>
       </c>
@@ -7847,7 +7905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="0" t="n">
         <v>2517</v>
       </c>
@@ -7862,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="0" t="n">
         <v>2537</v>
       </c>
@@ -7877,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="0" t="n">
         <v>2557</v>
       </c>
@@ -7892,7 +7950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="0" t="n">
         <v>2597</v>
       </c>
@@ -7907,7 +7965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="0" t="n">
         <v>1517</v>
       </c>
@@ -7922,7 +7980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="0" t="n">
         <v>1537</v>
       </c>
@@ -7937,7 +7995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="0" t="n">
         <v>1557</v>
       </c>
@@ -7952,7 +8010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="0" t="n">
         <v>1597</v>
       </c>
@@ -7967,7 +8025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="0" t="n">
         <v>517</v>
       </c>
@@ -7982,7 +8040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="n">
         <v>537</v>
       </c>
@@ -7997,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="n">
         <v>557</v>
       </c>
@@ -8012,7 +8070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="n">
         <v>597</v>
       </c>
@@ -8027,7 +8085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="n">
         <v>4518</v>
       </c>
@@ -8042,7 +8100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="n">
         <v>4538</v>
       </c>
@@ -8057,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="n">
         <v>4558</v>
       </c>
@@ -8072,7 +8130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="n">
         <v>4598</v>
       </c>
@@ -8087,7 +8145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="n">
         <v>3518</v>
       </c>
@@ -8102,7 +8160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="n">
         <v>3538</v>
       </c>
@@ -8117,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="n">
         <v>3558</v>
       </c>
@@ -8132,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="n">
         <v>3598</v>
       </c>
@@ -8147,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="n">
         <v>2518</v>
       </c>
@@ -8162,7 +8220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="n">
         <v>2538</v>
       </c>
@@ -8177,7 +8235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="n">
         <v>2558</v>
       </c>
@@ -8192,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="n">
         <v>2598</v>
       </c>
@@ -8207,7 +8265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="n">
         <v>1518</v>
       </c>
@@ -8222,7 +8280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="n">
         <v>1538</v>
       </c>
@@ -8237,7 +8295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="n">
         <v>1558</v>
       </c>
@@ -8252,7 +8310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="n">
         <v>1598</v>
       </c>
@@ -8267,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="n">
         <v>518</v>
       </c>
@@ -8282,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="0" t="n">
         <v>538</v>
       </c>
@@ -8297,7 +8355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B298" s="0" t="n">
         <v>558</v>
       </c>
@@ -8312,7 +8370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="0" t="n">
         <v>598</v>
       </c>
@@ -8327,7 +8385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="0" t="n">
         <v>6007</v>
       </c>
@@ -8339,7 +8397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="0" t="n">
         <v>6008</v>
       </c>
@@ -8351,7 +8409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="n">
         <v>6009</v>
       </c>
@@ -8363,7 +8421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="0" t="n">
         <v>6010</v>
       </c>
@@ -8375,7 +8433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B304" s="0" t="n">
         <v>7003</v>
       </c>
@@ -8387,7 +8445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B305" s="0" t="n">
         <v>7004</v>
       </c>
@@ -8399,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="0" t="n">
         <v>7005</v>
       </c>
@@ -8411,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="0" t="n">
         <v>107001</v>
       </c>
@@ -8432,7 +8490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="0" t="n">
         <v>107002</v>
       </c>
@@ -8483,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="0" t="n">
         <v>107004</v>
       </c>
@@ -8525,7 +8583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="0" t="n">
         <v>107006</v>
       </c>
@@ -8546,7 +8604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="0" t="n">
         <v>107007</v>
       </c>
@@ -8564,7 +8622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="n">
         <v>107009</v>
       </c>
@@ -8585,7 +8643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="0" t="n">
         <v>107301</v>
       </c>
@@ -8636,7 +8694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="0" t="n">
         <v>107303</v>
       </c>
@@ -8660,7 +8718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="0" t="n">
         <v>107304</v>
       </c>
@@ -8708,7 +8766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="0" t="n">
         <v>107306</v>
       </c>
@@ -8729,7 +8787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="n">
         <v>107307</v>
       </c>
@@ -8747,7 +8805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="0" t="n">
         <v>107308</v>
       </c>
@@ -8765,7 +8823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="n">
         <v>107309</v>
       </c>
@@ -8786,7 +8844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="0" t="n">
         <v>107310</v>
       </c>
@@ -8807,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="n">
         <v>107311</v>
       </c>
@@ -8822,7 +8880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="0" t="n">
         <v>107701</v>
       </c>
@@ -8846,7 +8904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="n">
         <v>107702</v>
       </c>
@@ -8870,7 +8928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="n">
         <v>107703</v>
       </c>
@@ -8891,7 +8949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="0" t="n">
         <v>108001</v>
       </c>
@@ -8915,7 +8973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="0" t="n">
         <v>108002</v>
       </c>
@@ -8939,7 +8997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="0" t="n">
         <v>108003</v>
       </c>
@@ -8960,7 +9018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B332" s="0" t="n">
         <v>108502</v>
       </c>
@@ -8978,7 +9036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B333" s="0" t="n">
         <v>108511</v>
       </c>
@@ -8999,7 +9057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="0" t="n">
         <v>108512</v>
       </c>
@@ -9020,7 +9078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="0" t="n">
         <v>108513</v>
       </c>
@@ -9041,7 +9099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="0" t="n">
         <v>108514</v>
       </c>
@@ -9062,7 +9120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B337" s="0" t="n">
         <v>108515</v>
       </c>
@@ -9083,7 +9141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B338" s="0" t="n">
         <v>108516</v>
       </c>
@@ -9104,7 +9162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B339" s="0" t="n">
         <v>108517</v>
       </c>
@@ -9125,7 +9183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B340" s="0" t="n">
         <v>108518</v>
       </c>
@@ -9149,7 +9207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B341" s="0" t="n">
         <v>108519</v>
       </c>
@@ -9167,7 +9225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="0" t="n">
         <v>108520</v>
       </c>
@@ -9185,7 +9243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B343" s="0" t="n">
         <v>110501</v>
       </c>
@@ -9206,7 +9264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B344" s="0" t="n">
         <v>110502</v>
       </c>
@@ -9227,7 +9285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B345" s="0" t="n">
         <v>110503</v>
       </c>
@@ -9248,7 +9306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="0" t="n">
         <v>110504</v>
       </c>
@@ -9269,7 +9327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B347" s="0" t="n">
         <v>110505</v>
       </c>
@@ -9287,7 +9345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="0" t="n">
         <v>110506</v>
       </c>
@@ -9305,7 +9363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="114.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B349" s="0" t="n">
         <v>110507</v>
       </c>
@@ -9332,7 +9390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B350" s="0" t="n">
         <v>110801</v>
       </c>
@@ -9356,7 +9414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="114.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B351" s="0" t="n">
         <v>110802</v>
       </c>
@@ -9380,7 +9438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B352" s="0" t="n">
         <v>110803</v>
       </c>
@@ -9398,7 +9456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="153" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="0" t="n">
         <v>110804</v>
       </c>
@@ -9425,7 +9483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="204" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B354" s="0" t="n">
         <v>110805</v>
       </c>
@@ -9452,7 +9510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B355" s="0" t="n">
         <v>110901</v>
       </c>
@@ -9479,7 +9537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B356" s="0" t="n">
         <v>110902</v>
       </c>
@@ -9506,7 +9564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B357" s="0" t="n">
         <v>110903</v>
       </c>
@@ -9533,7 +9591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B358" s="0" t="n">
         <v>111101</v>
       </c>
@@ -9560,7 +9618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="0" t="n">
         <v>111102</v>
       </c>
@@ -9587,7 +9645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B360" s="0" t="n">
         <v>111103</v>
       </c>
@@ -9614,7 +9672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B361" s="0" t="n">
         <v>110851</v>
       </c>
@@ -9632,7 +9690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B362" s="0" t="n">
         <v>110852</v>
       </c>
@@ -9656,7 +9714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="204" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="0" t="n">
         <v>110853</v>
       </c>
@@ -9683,7 +9741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B364" s="0" t="n">
         <v>110951</v>
       </c>
@@ -9701,7 +9759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B365" s="0" t="n">
         <v>110952</v>
       </c>
@@ -9725,7 +9783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B366" s="0" t="n">
         <v>110953</v>
       </c>
@@ -9752,7 +9810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B367" s="0" t="n">
         <v>111151</v>
       </c>
@@ -9770,7 +9828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="0" t="n">
         <v>111152</v>
       </c>
@@ -9794,7 +9852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="0" t="n">
         <v>111153</v>
       </c>
@@ -9821,7 +9879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="0" t="n">
         <v>111251</v>
       </c>
@@ -9839,7 +9897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="0" t="n">
         <v>111252</v>
       </c>
@@ -9863,7 +9921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="0" t="n">
         <v>111253</v>
       </c>
@@ -9890,7 +9948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="0" t="n">
         <v>111351</v>
       </c>
@@ -9908,7 +9966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" customFormat="false" ht="76.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B374" s="0" t="n">
         <v>111352</v>
       </c>
@@ -9932,7 +9990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="204" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B375" s="0" t="n">
         <v>11353</v>
       </c>
@@ -10046,7 +10104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="0" t="n">
         <v>115100</v>
       </c>
@@ -10070,7 +10128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="0" t="n">
         <v>115101</v>
       </c>
@@ -10094,7 +10152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="0" t="n">
         <v>115102</v>
       </c>
@@ -10118,7 +10176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="0" t="n">
         <v>115103</v>
       </c>
@@ -10142,7 +10200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="0" t="n">
         <v>115104</v>
       </c>
@@ -10235,7 +10293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="0" t="n">
         <v>108408</v>
       </c>
@@ -10280,7 +10338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
         <v>523</v>
       </c>
@@ -10293,208 +10351,276 @@
       <c r="E390" s="0" t="n">
         <v>2.662</v>
       </c>
-      <c r="L390" s="0" t="s">
+    </row>
+    <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
         <v>525</v>
-      </c>
-      <c r="N390" s="0" t="n">
-        <f aca="false">AND(E390 &gt; 0, K390 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="0" t="s">
-        <v>526</v>
       </c>
       <c r="B391" s="0" t="n">
         <v>170001</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E391" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="L391" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N391" s="0" t="n">
-        <f aca="false">AND(E391 &gt; 0, K391 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B392" s="0" t="n">
         <v>170002</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E392" s="9" t="n">
         <v>3.9</v>
       </c>
-      <c r="L392" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N392" s="0" t="n">
-        <f aca="false">AND(E392 &gt; 0, K392 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B393" s="0" t="n">
         <v>170003</v>
       </c>
       <c r="C393" s="0" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E393" s="9" t="n">
         <v>7.93</v>
       </c>
-      <c r="L393" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N393" s="0" t="n">
-        <f aca="false">AND(E393 &gt; 0, K393 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B394" s="0" t="n">
         <v>170004</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E394" s="9" t="n">
         <v>8.92</v>
       </c>
-      <c r="L394" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N394" s="0" t="n">
-        <f aca="false">AND(E394 &gt; 0, K394 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B395" s="0" t="n">
         <v>170005</v>
       </c>
       <c r="C395" s="0" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E395" s="9" t="n">
         <v>1.636</v>
       </c>
-      <c r="L395" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N395" s="0" t="n">
-        <f aca="false">AND(E395 &gt; 0, K395 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="396" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B396" s="0" t="n">
         <v>170006</v>
       </c>
       <c r="C396" s="0" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E396" s="9" t="n">
         <v>1.801</v>
       </c>
-      <c r="L396" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N396" s="0" t="n">
-        <f aca="false">AND(E396 &gt; 0, K396 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B397" s="0" t="n">
         <v>170007</v>
       </c>
       <c r="C397" s="0" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E397" s="9" t="n">
         <v>5.19</v>
       </c>
-      <c r="L397" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N397" s="0" t="n">
-        <f aca="false">AND(E397 &gt; 0, K397 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B398" s="0" t="n">
         <v>170008</v>
       </c>
       <c r="C398" s="0" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E398" s="9" t="n">
         <v>2.906</v>
       </c>
       <c r="H398" s="0" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="L398" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N398" s="0" t="n">
-        <f aca="false">AND(E398 &gt; 0, K398 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="0" t="s">
+      <c r="B399" s="0" t="n">
+        <v>170009</v>
+      </c>
+      <c r="C399" s="0" t="s">
         <v>543</v>
-      </c>
-      <c r="B399" s="0" t="n">
-        <v>170010</v>
-      </c>
-      <c r="C399" s="0" t="s">
-        <v>544</v>
       </c>
       <c r="E399" s="9" t="n">
         <v>4.1</v>
       </c>
-      <c r="L399" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="N399" s="0" t="n">
-        <f aca="false">AND(E399 &gt; 0, K399 = "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B400" s="0" t="n">
+        <v>170010</v>
+      </c>
+      <c r="E400" s="0" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="H400" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="I400" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="B401" s="0" t="n">
+        <v>170011</v>
+      </c>
+      <c r="E401" s="9" t="n">
+        <v>7.86</v>
+      </c>
+      <c r="H401" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="I401" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="B402" s="0" t="n">
+        <v>170012</v>
+      </c>
+      <c r="C402" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="E402" s="9" t="n">
+        <v>0.971</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="B403" s="0" t="n">
+        <v>114102</v>
+      </c>
+      <c r="C403" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="E403" s="0" t="n">
+        <v>2.32</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="B404" s="0" t="n">
+        <v>170014</v>
+      </c>
+      <c r="C404" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="E404" s="0" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="B405" s="0" t="n">
+        <v>170015</v>
+      </c>
+      <c r="C405" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="E405" s="0" t="n">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="B406" s="0" t="n">
+        <v>170016</v>
+      </c>
+      <c r="C406" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="E406" s="0" t="n">
+        <v>3.042</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="B407" s="0" t="n">
+        <v>114102</v>
+      </c>
+      <c r="C407" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="E407" s="0" t="n">
+        <v>2.32</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="B408" s="0" t="n">
+        <v>170017</v>
+      </c>
+      <c r="C408" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="E408" s="0" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="H408" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="I408" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:N389"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -10502,5 +10628,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>